<commit_message>
More work on aerodynamic debug
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/AERODYNAMIC_AND_STABILITY_CLIMB/Aerodynamic_and_Stability_CLIMB.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/AERODYNAMIC_AND_STABILITY_CLIMB/Aerodynamic_and_Stability_CLIMB.xlsx
@@ -795,7 +795,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.5667428199062847</v>
+        <v>1.5668648866206438</v>
       </c>
     </row>
     <row r="13">
@@ -828,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="n">
-        <v>18.18108149480034</v>
+        <v>18.18238357813309</v>
       </c>
     </row>
     <row r="16">
@@ -1039,37 +1039,37 @@
         <v>1.1825263624513955</v>
       </c>
       <c r="Z20" t="n">
-        <v>1.2677511106069694</v>
+        <v>1.2677511106214752</v>
       </c>
       <c r="AA20" t="n">
-        <v>1.3515240912901625</v>
+        <v>1.3515256841975578</v>
       </c>
       <c r="AB20" t="n">
-        <v>1.4275782169705309</v>
+        <v>1.4275890681636803</v>
       </c>
       <c r="AC20" t="n">
-        <v>1.4900933594472612</v>
+        <v>1.4901245610154703</v>
       </c>
       <c r="AD20" t="n">
-        <v>1.5351270947972182</v>
+        <v>1.5351887667593722</v>
       </c>
       <c r="AE20" t="n">
-        <v>1.5606147033749167</v>
+        <v>1.5607115949126324</v>
       </c>
       <c r="AF20" t="n">
-        <v>1.5663691698125355</v>
+        <v>1.5664962605032713</v>
       </c>
       <c r="AG20" t="n">
-        <v>1.5540811830198997</v>
+        <v>1.554219284070136</v>
       </c>
       <c r="AH20" t="n">
-        <v>1.5273191361845413</v>
+        <v>1.5274304916628552</v>
       </c>
       <c r="AI20" t="n">
-        <v>1.4915291267715922</v>
+        <v>1.4915530148418483</v>
       </c>
       <c r="AJ20" t="n">
-        <v>1.4540349565239516</v>
+        <v>1.4538832906784194</v>
       </c>
     </row>
     <row r="21">
@@ -7293,37 +7293,37 @@
         <v>1.1825263624513955</v>
       </c>
       <c r="Z81" t="n">
-        <v>1.2677511106069694</v>
+        <v>1.2677511106214752</v>
       </c>
       <c r="AA81" t="n">
-        <v>1.3515240912901625</v>
+        <v>1.3515256841975578</v>
       </c>
       <c r="AB81" t="n">
-        <v>1.4275782169705309</v>
+        <v>1.4275890681636803</v>
       </c>
       <c r="AC81" t="n">
-        <v>1.4900933594472612</v>
+        <v>1.4901245610154703</v>
       </c>
       <c r="AD81" t="n">
-        <v>1.5351270947972182</v>
+        <v>1.5351887667593722</v>
       </c>
       <c r="AE81" t="n">
-        <v>1.5606147033749167</v>
+        <v>1.5607115949126324</v>
       </c>
       <c r="AF81" t="n">
-        <v>1.5663691698125355</v>
+        <v>1.5664962605032713</v>
       </c>
       <c r="AG81" t="n">
-        <v>1.5540811830198997</v>
+        <v>1.554219284070136</v>
       </c>
       <c r="AH81" t="n">
-        <v>1.5273191361845413</v>
+        <v>1.5274304916628552</v>
       </c>
       <c r="AI81" t="n">
-        <v>1.4915291267715922</v>
+        <v>1.4915530148418483</v>
       </c>
       <c r="AJ81" t="n">
-        <v>1.4540349565239516</v>
+        <v>1.4538832906784194</v>
       </c>
     </row>
     <row r="82">
@@ -11529,7 +11529,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>1.7028562961589264</v>
+        <v>1.7029471006326313</v>
       </c>
     </row>
     <row r="13">
@@ -11562,7 +11562,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="n">
-        <v>26.312233812045125</v>
+        <v>26.31353589537787</v>
       </c>
     </row>
     <row r="16">
@@ -11660,40 +11660,40 @@
         <v>6.689646499744944</v>
       </c>
       <c r="Y19" t="n">
-        <v>7.29361078436979</v>
+        <v>7.293610784365219</v>
       </c>
       <c r="Z19" t="n">
-        <v>7.892703978881972</v>
+        <v>7.892703703634629</v>
       </c>
       <c r="AA19" t="n">
-        <v>8.491437019333887</v>
+        <v>8.491431408983917</v>
       </c>
       <c r="AB19" t="n">
-        <v>9.111014103893766</v>
+        <v>9.110978203547809</v>
       </c>
       <c r="AC19" t="n">
-        <v>9.765666350351346</v>
+        <v>9.765568625997542</v>
       </c>
       <c r="AD19" t="n">
-        <v>10.46648316863146</v>
+        <v>10.466293735665054</v>
       </c>
       <c r="AE19" t="n">
-        <v>11.26349334453808</v>
+        <v>11.263142154294478</v>
       </c>
       <c r="AF19" t="n">
-        <v>12.239839641222787</v>
+        <v>12.239391337760921</v>
       </c>
       <c r="AG19" t="n">
-        <v>13.277455980558418</v>
+        <v>13.276983683389279</v>
       </c>
       <c r="AH19" t="n">
-        <v>14.362744618225541</v>
+        <v>14.362371948370988</v>
       </c>
       <c r="AI19" t="n">
-        <v>15.47861827535596</v>
+        <v>15.478548558054698</v>
       </c>
       <c r="AJ19" t="n">
-        <v>16.585365919349613</v>
+        <v>16.585809357132305</v>
       </c>
     </row>
     <row r="20">
@@ -11770,40 +11770,40 @@
         <v>0.46652146940636585</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.5086406315389076</v>
+        <v>0.5086406315385888</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.5504200943888254</v>
+        <v>0.5504200751936714</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.5921744408740124</v>
+        <v>0.5921740496203473</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.6353824058853784</v>
+        <v>0.6353799022729456</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.6810364367791204</v>
+        <v>0.6810296216941776</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.7299098850041048</v>
+        <v>0.7298966743589916</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.7854943396566798</v>
+        <v>0.7854698375207888</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.8538374268522997</v>
+        <v>0.8538058754287897</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.9273873052023949</v>
+        <v>0.9273534501064961</v>
       </c>
       <c r="AH20" t="n">
-        <v>1.0057782215701043</v>
+        <v>1.005750849638122</v>
       </c>
       <c r="AI20" t="n">
-        <v>1.0880282558013807</v>
+        <v>1.0880229053101167</v>
       </c>
       <c r="AJ20" t="n">
-        <v>1.1709196608464776</v>
+        <v>1.1709532098612825</v>
       </c>
     </row>
     <row r="21">
@@ -18024,40 +18024,40 @@
         <v>0.46652146940636585</v>
       </c>
       <c r="Y81" t="n">
-        <v>0.5086406315389076</v>
+        <v>0.5086406315385888</v>
       </c>
       <c r="Z81" t="n">
-        <v>0.5504200943888254</v>
+        <v>0.5504200751936714</v>
       </c>
       <c r="AA81" t="n">
-        <v>0.5921744408740124</v>
+        <v>0.5921740496203473</v>
       </c>
       <c r="AB81" t="n">
-        <v>0.6353824058853784</v>
+        <v>0.6353799022729456</v>
       </c>
       <c r="AC81" t="n">
-        <v>0.6810364367791204</v>
+        <v>0.6810296216941776</v>
       </c>
       <c r="AD81" t="n">
-        <v>0.7299098850041048</v>
+        <v>0.7298966743589916</v>
       </c>
       <c r="AE81" t="n">
-        <v>0.7854943396566798</v>
+        <v>0.7854698375207888</v>
       </c>
       <c r="AF81" t="n">
-        <v>0.8538374268522997</v>
+        <v>0.8538058754287897</v>
       </c>
       <c r="AG81" t="n">
-        <v>0.9273873052023949</v>
+        <v>0.9273534501064961</v>
       </c>
       <c r="AH81" t="n">
-        <v>1.0057782215701043</v>
+        <v>1.005750849638122</v>
       </c>
       <c r="AI81" t="n">
-        <v>1.0880282558013807</v>
+        <v>1.0880229053101167</v>
       </c>
       <c r="AJ81" t="n">
-        <v>1.1709196608464776</v>
+        <v>1.1709532098612825</v>
       </c>
     </row>
     <row r="82">
@@ -18134,40 +18134,40 @@
         <v>0.00630660898157837</v>
       </c>
       <c r="Y82" t="n">
-        <v>0.006448743883997675</v>
+        <v>0.0064487438839965095</v>
       </c>
       <c r="Z82" t="n">
-        <v>0.006609984851111815</v>
+        <v>0.006609984773851376</v>
       </c>
       <c r="AA82" t="n">
-        <v>0.006781781761183724</v>
+        <v>0.006781780076340141</v>
       </c>
       <c r="AB82" t="n">
-        <v>0.006974212764990933</v>
+        <v>0.006974201328336692</v>
       </c>
       <c r="AC82" t="n">
-        <v>0.007188168806684497</v>
+        <v>0.007188135458806586</v>
       </c>
       <c r="AD82" t="n">
-        <v>0.007434073546217598</v>
+        <v>0.007434005597324457</v>
       </c>
       <c r="AE82" t="n">
-        <v>0.007732094643072676</v>
+        <v>0.007731957197527502</v>
       </c>
       <c r="AF82" t="n">
-        <v>0.008127383537643277</v>
+        <v>0.008127191375901182</v>
       </c>
       <c r="AG82" t="n">
-        <v>0.0085895197105053</v>
+        <v>0.008589299096269458</v>
       </c>
       <c r="AH82" t="n">
-        <v>0.009112149536845696</v>
+        <v>0.009111964062900265</v>
       </c>
       <c r="AI82" t="n">
-        <v>0.009688615434911063</v>
+        <v>0.009688578644183286</v>
       </c>
       <c r="AJ82" t="n">
-        <v>0.01030224719870613</v>
+        <v>0.010302499821997503</v>
       </c>
     </row>
     <row r="83">
@@ -20574,40 +20574,40 @@
         <v>6.689646499744944</v>
       </c>
       <c r="Y117" t="n">
-        <v>7.29361078436979</v>
+        <v>7.293610784365219</v>
       </c>
       <c r="Z117" t="n">
-        <v>7.892703978881972</v>
+        <v>7.892703703634629</v>
       </c>
       <c r="AA117" t="n">
-        <v>8.491437019333887</v>
+        <v>8.491431408983917</v>
       </c>
       <c r="AB117" t="n">
-        <v>9.111014103893766</v>
+        <v>9.110978203547809</v>
       </c>
       <c r="AC117" t="n">
-        <v>9.765666350351346</v>
+        <v>9.765568625997542</v>
       </c>
       <c r="AD117" t="n">
-        <v>10.46648316863146</v>
+        <v>10.466293735665054</v>
       </c>
       <c r="AE117" t="n">
-        <v>11.26349334453808</v>
+        <v>11.263142154294478</v>
       </c>
       <c r="AF117" t="n">
-        <v>12.239839641222787</v>
+        <v>12.239391337760921</v>
       </c>
       <c r="AG117" t="n">
-        <v>13.277455980558418</v>
+        <v>13.276983683389279</v>
       </c>
       <c r="AH117" t="n">
-        <v>14.362744618225541</v>
+        <v>14.362371948370988</v>
       </c>
       <c r="AI117" t="n">
-        <v>15.47861827535596</v>
+        <v>15.478548558054698</v>
       </c>
       <c r="AJ117" t="n">
-        <v>16.585365919349613</v>
+        <v>16.585809357132305</v>
       </c>
     </row>
     <row r="118">
@@ -20684,40 +20684,40 @@
         <v>0.004203026916624806</v>
       </c>
       <c r="Y118" t="n">
-        <v>0.004582490636427467</v>
+        <v>0.004582490636424631</v>
       </c>
       <c r="Z118" t="n">
-        <v>0.004958893907093196</v>
+        <v>0.00495889373415851</v>
       </c>
       <c r="AA118" t="n">
-        <v>0.005335070897161038</v>
+        <v>0.005335067372243529</v>
       </c>
       <c r="AB118" t="n">
-        <v>0.005724343957169293</v>
+        <v>0.0057243214014004</v>
       </c>
       <c r="AC118" t="n">
-        <v>0.006135654332537395</v>
+        <v>0.0061355929334650575</v>
       </c>
       <c r="AD118" t="n">
-        <v>0.006575969370255323</v>
+        <v>0.006575850351730686</v>
       </c>
       <c r="AE118" t="n">
-        <v>0.007076721573273413</v>
+        <v>0.0070765009245370115</v>
       </c>
       <c r="AF118" t="n">
-        <v>0.007690148570509999</v>
+        <v>0.007689866906670594</v>
       </c>
       <c r="AG118" t="n">
-        <v>0.008342070821337942</v>
+        <v>0.008341774082531995</v>
       </c>
       <c r="AH118" t="n">
-        <v>0.00902394502150615</v>
+        <v>0.009023710877380653</v>
       </c>
       <c r="AI118" t="n">
-        <v>0.009725035432883057</v>
+        <v>0.009724991630315314</v>
       </c>
       <c r="AJ118" t="n">
-        <v>0.010420392076585168</v>
+        <v>0.010420670683374931</v>
       </c>
     </row>
     <row r="119">
@@ -22163,7 +22163,7 @@
         <v>5</v>
       </c>
       <c r="C154" t="n">
-        <v>23.916696733985745</v>
+        <v>23.917998817318484</v>
       </c>
     </row>
     <row r="155">
@@ -22174,7 +22174,7 @@
         <v>5</v>
       </c>
       <c r="C155" t="n">
-        <v>8.604462921940616</v>
+        <v>8.604462921940609</v>
       </c>
     </row>
     <row r="156">
@@ -22185,7 +22185,7 @@
         <v>5</v>
       </c>
       <c r="C156" t="n">
-        <v>1.7170751795049968</v>
+        <v>1.7171659839787017</v>
       </c>
     </row>
     <row r="157">
@@ -22196,7 +22196,7 @@
         <v>5</v>
       </c>
       <c r="C157" t="n">
-        <v>0.7813350775523988</v>
+        <v>0.7813350775523984</v>
       </c>
     </row>
     <row r="158">
@@ -22294,40 +22294,40 @@
         <v>6.689646499744944</v>
       </c>
       <c r="Y161" t="n">
-        <v>7.29361078436979</v>
+        <v>7.293610784365219</v>
       </c>
       <c r="Z161" t="n">
-        <v>7.892703978881972</v>
+        <v>7.892703703634629</v>
       </c>
       <c r="AA161" t="n">
-        <v>8.491437019333887</v>
+        <v>8.491431408983917</v>
       </c>
       <c r="AB161" t="n">
-        <v>9.111014103893766</v>
+        <v>9.110978203547809</v>
       </c>
       <c r="AC161" t="n">
-        <v>9.765666350351346</v>
+        <v>9.765568625997542</v>
       </c>
       <c r="AD161" t="n">
-        <v>10.46648316863146</v>
+        <v>10.466293735665054</v>
       </c>
       <c r="AE161" t="n">
-        <v>11.26349334453808</v>
+        <v>11.263142154294478</v>
       </c>
       <c r="AF161" t="n">
-        <v>12.239839641222787</v>
+        <v>12.239391337760921</v>
       </c>
       <c r="AG161" t="n">
-        <v>13.277455980558418</v>
+        <v>13.276983683389279</v>
       </c>
       <c r="AH161" t="n">
-        <v>14.362744618225541</v>
+        <v>14.362371948370988</v>
       </c>
       <c r="AI161" t="n">
-        <v>15.47861827535596</v>
+        <v>15.478548558054698</v>
       </c>
       <c r="AJ161" t="n">
-        <v>16.585365919349613</v>
+        <v>16.585809357132305</v>
       </c>
     </row>
     <row r="162">
@@ -22404,40 +22404,40 @@
         <v>0.6477999242434423</v>
       </c>
       <c r="Y162" t="n">
-        <v>0.6899190863759841</v>
+        <v>0.6899190863756653</v>
       </c>
       <c r="Z162" t="n">
-        <v>0.7316985492259019</v>
+        <v>0.7316985300307479</v>
       </c>
       <c r="AA162" t="n">
-        <v>0.7734528957110889</v>
+        <v>0.7734525044574238</v>
       </c>
       <c r="AB162" t="n">
-        <v>0.8166795860186467</v>
+        <v>0.8166770769526452</v>
       </c>
       <c r="AC162" t="n">
-        <v>0.8625279414629908</v>
+        <v>0.8625210586019285</v>
       </c>
       <c r="AD162" t="n">
-        <v>0.9120115066683677</v>
+        <v>0.9119980056784254</v>
       </c>
       <c r="AE162" t="n">
-        <v>0.9689842651110688</v>
+        <v>0.9689588573348553</v>
       </c>
       <c r="AF162" t="n">
-        <v>1.0399436847059749</v>
+        <v>1.0399106137008165</v>
       </c>
       <c r="AG162" t="n">
-        <v>1.116726836794431</v>
+        <v>1.1166914689557164</v>
       </c>
       <c r="AH162" t="n">
-        <v>1.1981629331787762</v>
+        <v>1.1981351130562432</v>
       </c>
       <c r="AI162" t="n">
-        <v>1.282253910379203</v>
+        <v>1.282250023697285</v>
       </c>
       <c r="AJ162" t="n">
-        <v>1.3647267664676934</v>
+        <v>1.3647629356199695</v>
       </c>
     </row>
     <row r="163">
@@ -22529,40 +22529,40 @@
         <v>0.6477999242434423</v>
       </c>
       <c r="Y166" t="n">
-        <v>0.6899190863759841</v>
+        <v>0.6899190863756653</v>
       </c>
       <c r="Z166" t="n">
-        <v>0.7316985492259019</v>
+        <v>0.7316985300307479</v>
       </c>
       <c r="AA166" t="n">
-        <v>0.7734528957110889</v>
+        <v>0.7734525044574238</v>
       </c>
       <c r="AB166" t="n">
-        <v>0.8166795860186467</v>
+        <v>0.8166770769526452</v>
       </c>
       <c r="AC166" t="n">
-        <v>0.8625279414629908</v>
+        <v>0.8625210586019285</v>
       </c>
       <c r="AD166" t="n">
-        <v>0.9120115066683677</v>
+        <v>0.9119980056784254</v>
       </c>
       <c r="AE166" t="n">
-        <v>0.9689842651110688</v>
+        <v>0.9689588573348553</v>
       </c>
       <c r="AF166" t="n">
-        <v>1.0399436847059749</v>
+        <v>1.0399106137008165</v>
       </c>
       <c r="AG166" t="n">
-        <v>1.116726836794431</v>
+        <v>1.1166914689557164</v>
       </c>
       <c r="AH166" t="n">
-        <v>1.1981629331787762</v>
+        <v>1.1981351130562432</v>
       </c>
       <c r="AI166" t="n">
-        <v>1.282253910379203</v>
+        <v>1.282250023697285</v>
       </c>
       <c r="AJ166" t="n">
-        <v>1.3647267664676934</v>
+        <v>1.3647629356199695</v>
       </c>
     </row>
     <row r="167">
@@ -22639,40 +22639,40 @@
         <v>0.00670660898157837</v>
       </c>
       <c r="Y167" t="n">
-        <v>0.006848743883997675</v>
+        <v>0.00684874388399651</v>
       </c>
       <c r="Z167" t="n">
-        <v>0.007009984851111815</v>
+        <v>0.0070099847738513766</v>
       </c>
       <c r="AA167" t="n">
-        <v>0.0071817817611837245</v>
+        <v>0.007181780076340141</v>
       </c>
       <c r="AB167" t="n">
-        <v>0.007374212764990933</v>
+        <v>0.007374201328336692</v>
       </c>
       <c r="AC167" t="n">
-        <v>0.007588168806684497</v>
+        <v>0.007588135458806586</v>
       </c>
       <c r="AD167" t="n">
-        <v>0.007834073546217598</v>
+        <v>0.007834005597324457</v>
       </c>
       <c r="AE167" t="n">
-        <v>0.008132094643072676</v>
+        <v>0.008131957197527502</v>
       </c>
       <c r="AF167" t="n">
-        <v>0.008527383537643277</v>
+        <v>0.008527191375901182</v>
       </c>
       <c r="AG167" t="n">
-        <v>0.0089895197105053</v>
+        <v>0.008989299096269457</v>
       </c>
       <c r="AH167" t="n">
-        <v>0.009512149536845696</v>
+        <v>0.009511964062900264</v>
       </c>
       <c r="AI167" t="n">
-        <v>0.010088615434911062</v>
+        <v>0.010088578644183286</v>
       </c>
       <c r="AJ167" t="n">
-        <v>0.01070224719870613</v>
+        <v>0.010702499821997502</v>
       </c>
     </row>
     <row r="168">
@@ -22764,40 +22764,40 @@
         <v>6.689646499744944</v>
       </c>
       <c r="Y171" t="n">
-        <v>7.29361078436979</v>
+        <v>7.293610784365219</v>
       </c>
       <c r="Z171" t="n">
-        <v>7.892703978881972</v>
+        <v>7.892703703634629</v>
       </c>
       <c r="AA171" t="n">
-        <v>8.491437019333887</v>
+        <v>8.491431408983917</v>
       </c>
       <c r="AB171" t="n">
-        <v>9.111014103893766</v>
+        <v>9.110978203547809</v>
       </c>
       <c r="AC171" t="n">
-        <v>9.765666350351346</v>
+        <v>9.765568625997542</v>
       </c>
       <c r="AD171" t="n">
-        <v>10.46648316863146</v>
+        <v>10.466293735665054</v>
       </c>
       <c r="AE171" t="n">
-        <v>11.26349334453808</v>
+        <v>11.263142154294478</v>
       </c>
       <c r="AF171" t="n">
-        <v>12.239839641222787</v>
+        <v>12.239391337760921</v>
       </c>
       <c r="AG171" t="n">
-        <v>13.277455980558418</v>
+        <v>13.276983683389279</v>
       </c>
       <c r="AH171" t="n">
-        <v>14.362744618225541</v>
+        <v>14.362371948370988</v>
       </c>
       <c r="AI171" t="n">
-        <v>15.47861827535596</v>
+        <v>15.478548558054698</v>
       </c>
       <c r="AJ171" t="n">
-        <v>16.585365919349613</v>
+        <v>16.585809357132305</v>
       </c>
     </row>
     <row r="172">
@@ -22874,40 +22874,40 @@
         <v>6.777431468130849E-4</v>
       </c>
       <c r="Y172" t="n">
-        <v>0.001057206866615746</v>
+        <v>0.0010572068666129097</v>
       </c>
       <c r="Z172" t="n">
-        <v>0.0014336101372814753</v>
+        <v>0.0014336099643467888</v>
       </c>
       <c r="AA172" t="n">
-        <v>0.001809787127349317</v>
+        <v>0.0018097836024318081</v>
       </c>
       <c r="AB172" t="n">
-        <v>0.0021990601873575722</v>
+        <v>0.002199037631588679</v>
       </c>
       <c r="AC172" t="n">
-        <v>0.002610370562725674</v>
+        <v>0.0026103091636533364</v>
       </c>
       <c r="AD172" t="n">
-        <v>0.003050685600443602</v>
+        <v>0.0030505665819189646</v>
       </c>
       <c r="AE172" t="n">
-        <v>0.0035514378034616923</v>
+        <v>0.0035512171547252905</v>
       </c>
       <c r="AF172" t="n">
-        <v>0.0041648648006982775</v>
+        <v>0.004164583136858873</v>
       </c>
       <c r="AG172" t="n">
-        <v>0.004816787051526221</v>
+        <v>0.004816490312720274</v>
       </c>
       <c r="AH172" t="n">
-        <v>0.0054986612516944285</v>
+        <v>0.005498427107568932</v>
       </c>
       <c r="AI172" t="n">
-        <v>0.006199751663071336</v>
+        <v>0.006199707860503593</v>
       </c>
       <c r="AJ172" t="n">
-        <v>0.0068951083067734465</v>
+        <v>0.00689538691356321</v>
       </c>
     </row>
     <row r="173">
@@ -36117,43 +36117,43 @@
         <v>0.32675189706483576</v>
       </c>
       <c r="X12" t="n">
-        <v>0.33273658411297014</v>
+        <v>0.33273658411548346</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.33831838647463447</v>
+        <v>0.3383185378606732</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.341195570769746</v>
+        <v>0.3411986564597149</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.3299294312435129</v>
+        <v>0.32994902504775026</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.2991738679403961</v>
+        <v>0.2992245306425069</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.2544920143942668</v>
+        <v>0.2545764573355133</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.1761951531972963</v>
+        <v>0.17633455943668358</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.02465394007476878</v>
+        <v>0.02479631884727338</v>
       </c>
       <c r="AF12" t="n">
-        <v>-0.10767944981118556</v>
+        <v>-0.10761284100213928</v>
       </c>
       <c r="AG12" t="n">
-        <v>-0.1675977373515128</v>
+        <v>-0.16763933583553695</v>
       </c>
       <c r="AH12" t="n">
-        <v>-0.21063926213864625</v>
+        <v>-0.21086068106597888</v>
       </c>
       <c r="AI12" t="n">
-        <v>-0.22244171561823234</v>
+        <v>-0.22289057481871627</v>
       </c>
       <c r="AJ12" t="n">
-        <v>-0.21742240839300883</v>
+        <v>-0.2179868789853586</v>
       </c>
     </row>
     <row r="13">
@@ -36230,40 +36230,40 @@
         <v>3.4012625911641416</v>
       </c>
       <c r="Y13" t="n">
-        <v>3.7063892156302067</v>
+        <v>3.7063892156347764</v>
       </c>
       <c r="Z13" t="n">
-        <v>4.016386930208931</v>
+        <v>4.016387205456274</v>
       </c>
       <c r="AA13" t="n">
-        <v>4.326744798847926</v>
+        <v>4.326750409197894</v>
       </c>
       <c r="AB13" t="n">
-        <v>4.616258623378954</v>
+        <v>4.6162945237249104</v>
       </c>
       <c r="AC13" t="n">
-        <v>4.870697286012282</v>
+        <v>4.870795010366088</v>
       </c>
       <c r="AD13" t="n">
-        <v>5.078971376823075</v>
+        <v>5.07916080978948</v>
       </c>
       <c r="AE13" t="n">
-        <v>5.191052110007366</v>
+        <v>5.1914033002509665</v>
       </c>
       <c r="AF13" t="n">
-        <v>5.123796722413564</v>
+        <v>5.124245025875432</v>
       </c>
       <c r="AG13" t="n">
-        <v>4.995271292168846</v>
+        <v>4.995743589337986</v>
       </c>
       <c r="AH13" t="n">
-        <v>4.819073563592632</v>
+        <v>4.819446233447183</v>
       </c>
       <c r="AI13" t="n">
-        <v>4.612290815553125</v>
+        <v>4.612360532854387</v>
       </c>
       <c r="AJ13" t="n">
-        <v>4.414634080650389</v>
+        <v>4.4141906428676965</v>
       </c>
     </row>
     <row r="14">
@@ -36617,40 +36617,40 @@
         <v>0.6477999242434423</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.6899190863759841</v>
+        <v>0.6899190863756653</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.7316985492259019</v>
+        <v>0.7316985300307479</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.7734528957110889</v>
+        <v>0.7734525044574238</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.8166795860186467</v>
+        <v>0.8166770769526452</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.8625279414629908</v>
+        <v>0.8625210586019285</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.9120115066683677</v>
+        <v>0.9119980056784254</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.9689842651110688</v>
+        <v>0.9689588573348553</v>
       </c>
       <c r="AF6" t="n">
-        <v>1.0399436847059749</v>
+        <v>1.0399106137008165</v>
       </c>
       <c r="AG6" t="n">
-        <v>1.116726836794431</v>
+        <v>1.1166914689557164</v>
       </c>
       <c r="AH6" t="n">
-        <v>1.1981629331787762</v>
+        <v>1.1981351130562432</v>
       </c>
       <c r="AI6" t="n">
-        <v>1.282253910379203</v>
+        <v>1.282250023697285</v>
       </c>
       <c r="AJ6" t="n">
-        <v>1.3647267664676934</v>
+        <v>1.3647629356199695</v>
       </c>
     </row>
     <row r="7">
@@ -36727,40 +36727,40 @@
         <v>1.248519611759036</v>
       </c>
       <c r="Y7" t="n">
-        <v>1.3439262005652444</v>
+        <v>1.3439262005651835</v>
       </c>
       <c r="Z7" t="n">
-        <v>1.4392015356919632</v>
+        <v>1.4392015904182818</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.5305909375279074</v>
+        <v>1.530594227387853</v>
       </c>
       <c r="AB7" t="n">
-        <v>1.610397008279838</v>
+        <v>1.610412205626445</v>
       </c>
       <c r="AC7" t="n">
-        <v>1.6735767747896018</v>
+        <v>1.673614190784913</v>
       </c>
       <c r="AD7" t="n">
-        <v>1.7183769845473402</v>
+        <v>1.7184441039936555</v>
       </c>
       <c r="AE7" t="n">
-        <v>1.7469017912467408</v>
+        <v>1.7469981249762283</v>
       </c>
       <c r="AF7" t="n">
-        <v>1.7650751875546025</v>
+        <v>1.7651901065753417</v>
       </c>
       <c r="AG7" t="n">
-        <v>1.7793404500390426</v>
+        <v>1.779447016812291</v>
       </c>
       <c r="AH7" t="n">
-        <v>1.8007901601095502</v>
+        <v>1.8008412038332178</v>
       </c>
       <c r="AI7" t="n">
-        <v>1.8436747228706345</v>
+        <v>1.8435986682691772</v>
       </c>
       <c r="AJ7" t="n">
-        <v>1.9251262387781092</v>
+        <v>1.924821243494153</v>
       </c>
     </row>
     <row r="8">
@@ -36837,40 +36837,40 @@
         <v>0.00670660898157837</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.006848743883997675</v>
+        <v>0.00684874388399651</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.007009984851111815</v>
+        <v>0.0070099847738513766</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.0071817817611837245</v>
+        <v>0.007181780076340141</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.007374212764990933</v>
+        <v>0.007374201328336692</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.007588168806684497</v>
+        <v>0.007588135458806586</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.007834073546217598</v>
+        <v>0.007834005597324457</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.008132094643072676</v>
+        <v>0.008131957197527502</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.008527383537643277</v>
+        <v>0.008527191375901182</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.0089895197105053</v>
+        <v>0.008989299096269457</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.009512149536845696</v>
+        <v>0.009511964062900264</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.010088615434911062</v>
+        <v>0.010088578644183286</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.01070224719870613</v>
+        <v>0.010702499821997502</v>
       </c>
     </row>
     <row r="9">
@@ -36947,40 +36947,40 @@
         <v>0.09150934630442253</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.10502457026273608</v>
+        <v>0.10502457026273586</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.11998387953107131</v>
+        <v>0.1199838795163346</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.13626142446897768</v>
+        <v>0.13626142414760936</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.1538286618197317</v>
+        <v>0.15382865963829584</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.17280474247584443</v>
+        <v>0.17280473611504552</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.19325869195089806</v>
+        <v>0.19325867899027588</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.21509113294729457</v>
+        <v>0.2150911067308295</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.2382724121108821</v>
+        <v>0.2382723754578092</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.2622373043800932</v>
+        <v>0.2622372622999705</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.27844943182974774</v>
+        <v>0.2784493964523101</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.28749799437947104</v>
+        <v>0.2874979873619804</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.29546783935530113</v>
+        <v>0.2954678875408547</v>
       </c>
     </row>
     <row r="10">
@@ -37057,40 +37057,40 @@
         <v>6.777431468130849E-4</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.001057206866615746</v>
+        <v>0.0010572068666129097</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.0014336101372814753</v>
+        <v>0.0014336099643467888</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.001809787127349317</v>
+        <v>0.0018097836024318081</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.0021990601873575722</v>
+        <v>0.002199037631588679</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.002610370562725674</v>
+        <v>0.0026103091636533364</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.003050685600443602</v>
+        <v>0.0030505665819189646</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.0035514378034616923</v>
+        <v>0.0035512171547252905</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.0041648648006982775</v>
+        <v>0.004164583136858873</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.004816787051526221</v>
+        <v>0.004816490312720274</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.0054986612516944285</v>
+        <v>0.005498427107568932</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.006199751663071336</v>
+        <v>0.006199707860503593</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.0068951083067734465</v>
+        <v>0.00689538691356321</v>
       </c>
     </row>
     <row r="11">
@@ -37177,40 +37177,40 @@
         <v>-0.4841236521160264</v>
       </c>
       <c r="Y13" t="n">
-        <v>-0.49930786674529054</v>
+        <v>-0.49930786674489486</v>
       </c>
       <c r="Z13" t="n">
-        <v>-0.5146705581958457</v>
+        <v>-0.514670538459131</v>
       </c>
       <c r="AA13" t="n">
-        <v>-0.5303104058334388</v>
+        <v>-0.5303101768668138</v>
       </c>
       <c r="AB13" t="n">
-        <v>-0.5473358247356426</v>
+        <v>-0.547333987229286</v>
       </c>
       <c r="AC13" t="n">
-        <v>-0.5664346041589456</v>
+        <v>-0.5664294195857174</v>
       </c>
       <c r="AD13" t="n">
-        <v>-0.588340680077149</v>
+        <v>-0.5883303321554062</v>
       </c>
       <c r="AE13" t="n">
-        <v>-0.6177079985033123</v>
+        <v>-0.6176862368058218</v>
       </c>
       <c r="AF13" t="n">
-        <v>-0.6628861167005128</v>
+        <v>-0.6628573962258247</v>
       </c>
       <c r="AG13" t="n">
-        <v>-0.7144631335167346</v>
+        <v>-0.7144313013439165</v>
       </c>
       <c r="AH13" t="n">
-        <v>-0.7751982285058578</v>
+        <v>-0.7751698319434814</v>
       </c>
       <c r="AI13" t="n">
-        <v>-0.8441515719587452</v>
+        <v>-0.8441374181710967</v>
       </c>
       <c r="AJ13" t="n">
-        <v>-0.9163217075782851</v>
+        <v>-0.9163271246016725</v>
       </c>
     </row>
     <row r="14">
@@ -37302,40 +37302,40 @@
         <v>0.46652146940636585</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.5086406315389076</v>
+        <v>0.5086406315385888</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.5504200943888254</v>
+        <v>0.5504200751936714</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.5921744408740124</v>
+        <v>0.5921740496203473</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.6353824058853784</v>
+        <v>0.6353799022729456</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.6810364367791204</v>
+        <v>0.6810296216941776</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.7299098850041048</v>
+        <v>0.7298966743589916</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.7854943396414966</v>
+        <v>0.785469837505647</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.8538374265527648</v>
+        <v>0.8538058751294755</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.9273873043230403</v>
+        <v>0.9273534492274882</v>
       </c>
       <c r="AH17" t="n">
-        <v>1.0057782199524492</v>
+        <v>1.0057508480207538</v>
       </c>
       <c r="AI17" t="n">
-        <v>1.0880282534781882</v>
+        <v>1.0880229029869055</v>
       </c>
       <c r="AJ17" t="n">
-        <v>1.1709196580757308</v>
+        <v>1.1709532070901725</v>
       </c>
     </row>
     <row r="18">
@@ -37412,40 +37412,40 @@
         <v>1.2139424251103843</v>
       </c>
       <c r="Y18" t="n">
-        <v>1.3093490139165926</v>
+        <v>1.3093490139165318</v>
       </c>
       <c r="Z18" t="n">
-        <v>1.4046243490433115</v>
+        <v>1.4046244037696303</v>
       </c>
       <c r="AA18" t="n">
-        <v>1.4960137508792557</v>
+        <v>1.4960170407392013</v>
       </c>
       <c r="AB18" t="n">
-        <v>1.5758162499543311</v>
+        <v>1.575831448341156</v>
       </c>
       <c r="AC18" t="n">
-        <v>1.638958950855484</v>
+        <v>1.6389963797784626</v>
       </c>
       <c r="AD18" t="n">
-        <v>1.683642786448805</v>
+        <v>1.683709961275708</v>
       </c>
       <c r="AE18" t="n">
-        <v>1.7119027870528296</v>
+        <v>1.7119992935248305</v>
       </c>
       <c r="AF18" t="n">
-        <v>1.7295771421281385</v>
+        <v>1.7296923509950484</v>
       </c>
       <c r="AG18" t="n">
-        <v>1.743225687476025</v>
+        <v>1.7433325427910238</v>
       </c>
       <c r="AH18" t="n">
-        <v>1.7640945575154492</v>
+        <v>1.7641456867273688</v>
       </c>
       <c r="AI18" t="n">
-        <v>1.8066279773174514</v>
+        <v>1.8065516435079125</v>
       </c>
       <c r="AJ18" t="n">
-        <v>1.888159327477331</v>
+        <v>1.8878538324263447</v>
       </c>
     </row>
     <row r="19">
@@ -37522,40 +37522,40 @@
         <v>0.00630660898157837</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.006448743883997675</v>
+        <v>0.0064487438839965095</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.006609984851111815</v>
+        <v>0.006609984773851376</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.006781781761183724</v>
+        <v>0.006781780076340141</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.006974212764990933</v>
+        <v>0.006974201328336692</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.007188168806684497</v>
+        <v>0.007188135458806586</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.007434073546217598</v>
+        <v>0.007434005597324457</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.007732094643072676</v>
+        <v>0.007731957197527502</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.008127383537643277</v>
+        <v>0.008127191375901182</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.0085895197105053</v>
+        <v>0.008589299096269458</v>
       </c>
       <c r="AH19" t="n">
-        <v>0.009112149536845696</v>
+        <v>0.009111964062900265</v>
       </c>
       <c r="AI19" t="n">
-        <v>0.009688615434911063</v>
+        <v>0.009688578644183286</v>
       </c>
       <c r="AJ19" t="n">
-        <v>0.01030224719870613</v>
+        <v>0.010302499821997503</v>
       </c>
     </row>
     <row r="20">
@@ -37632,40 +37632,40 @@
         <v>0.09143305000836302</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.10494827396667657</v>
+        <v>0.10494827396667634</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.1199075832350118</v>
+        <v>0.11990758322027509</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.13618512817291817</v>
+        <v>0.13618512785154985</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.15375236552367222</v>
+        <v>0.1537523633422363</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.17272844617978492</v>
+        <v>0.172728439818986</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.19318239565483855</v>
+        <v>0.19318238269421636</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.21501483665123503</v>
+        <v>0.21501481043477003</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.2381961158148226</v>
+        <v>0.23819607916174965</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.26216100808403364</v>
+        <v>0.26216096600391103</v>
       </c>
       <c r="AH20" t="n">
-        <v>0.27837313553368825</v>
+        <v>0.2783731001562506</v>
       </c>
       <c r="AI20" t="n">
-        <v>0.2874216980834115</v>
+        <v>0.28742169106592086</v>
       </c>
       <c r="AJ20" t="n">
-        <v>0.2953915430592416</v>
+        <v>0.2953915912447952</v>
       </c>
     </row>
     <row r="21">
@@ -37742,40 +37742,40 @@
         <v>0.004203018328486302</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.004582482048288963</v>
+        <v>0.0045824820482861265</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.004958885318954692</v>
+        <v>0.004958885146020006</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.005335062309022534</v>
+        <v>0.005335058784105025</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.005724335369030789</v>
+        <v>0.005724312813261896</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.006135645744398891</v>
+        <v>0.006135584345326553</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.006575960782116819</v>
+        <v>0.0065758417635921815</v>
       </c>
       <c r="AE21" t="n">
-        <v>0.007076712985134909</v>
+        <v>0.007076492336398507</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.007690139982371494</v>
+        <v>0.0076898583185320895</v>
       </c>
       <c r="AG21" t="n">
-        <v>0.008342062233199438</v>
+        <v>0.00834176549439349</v>
       </c>
       <c r="AH21" t="n">
-        <v>0.009023936433367645</v>
+        <v>0.009023702289242149</v>
       </c>
       <c r="AI21" t="n">
-        <v>0.009725026844744553</v>
+        <v>0.00972498304217681</v>
       </c>
       <c r="AJ21" t="n">
-        <v>0.010420383488446663</v>
+        <v>0.010420662095236427</v>
       </c>
     </row>
     <row r="22">
@@ -37862,40 +37862,40 @@
         <v>-0.25890774867087923</v>
       </c>
       <c r="Y24" t="n">
-        <v>-0.27347412092858375</v>
+        <v>-0.27347412092818796</v>
       </c>
       <c r="Z24" t="n">
-        <v>-0.28827570131683494</v>
+        <v>-0.28827568158012035</v>
       </c>
       <c r="AA24" t="n">
-        <v>-0.30341131045808967</v>
+        <v>-0.3034110814914647</v>
       </c>
       <c r="AB24" t="n">
-        <v>-0.31996605025716557</v>
+        <v>-0.31996421957752347</v>
       </c>
       <c r="AC24" t="n">
-        <v>-0.3384310003732082</v>
+        <v>-0.33842590078424023</v>
       </c>
       <c r="AD24" t="n">
-        <v>-0.35923766039008387</v>
+        <v>-0.359227677051258</v>
       </c>
       <c r="AE24" t="n">
-        <v>-0.38658281289009727</v>
+        <v>-0.38656218973271844</v>
       </c>
       <c r="AF24" t="n">
-        <v>-0.4282479080216295</v>
+        <v>-0.4282210996759884</v>
       </c>
       <c r="AG24" t="n">
-        <v>-0.4755887748897714</v>
+        <v>-0.475558847516204</v>
       </c>
       <c r="AH24" t="n">
-        <v>-0.5323802471043375</v>
+        <v>-0.5323524151257936</v>
       </c>
       <c r="AI24" t="n">
-        <v>-0.5989659591503876</v>
+        <v>-0.59894996110311</v>
       </c>
       <c r="AJ24" t="n">
-        <v>-0.6716763800502416</v>
+        <v>-0.6716784962340864</v>
       </c>
     </row>
     <row r="25">
@@ -37987,40 +37987,40 @@
         <v>0.28524301456928935</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.3273621767018311</v>
+        <v>0.32736217670151235</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.36914163955174895</v>
+        <v>0.3691416203565949</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.4108959860369359</v>
+        <v>0.41089559478327076</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.4541039510483019</v>
+        <v>0.4541014474358691</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.4997579819420439</v>
+        <v>0.4997511668571011</v>
       </c>
       <c r="AD28" t="n">
-        <v>0.5486314301670283</v>
+        <v>0.5486182195219151</v>
       </c>
       <c r="AE28" t="n">
-        <v>0.6042131949747741</v>
+        <v>0.6041887037272182</v>
       </c>
       <c r="AF28" t="n">
-        <v>0.6723014727329754</v>
+        <v>0.6722702090197467</v>
       </c>
       <c r="AG28" t="n">
-        <v>0.7446625906672891</v>
+        <v>0.7446296536848415</v>
       </c>
       <c r="AH28" t="n">
-        <v>0.8204735319568672</v>
+        <v>0.8204473925511997</v>
       </c>
       <c r="AI28" t="n">
-        <v>0.8992950093746845</v>
+        <v>0.8992899711562621</v>
       </c>
       <c r="AJ28" t="n">
-        <v>0.9789610674890019</v>
+        <v>0.978993158514168</v>
       </c>
     </row>
     <row r="29">
@@ -38097,40 +38097,40 @@
         <v>1.1793652384617328</v>
       </c>
       <c r="Y29" t="n">
-        <v>1.274771827267941</v>
+        <v>1.2747718272678803</v>
       </c>
       <c r="Z29" t="n">
-        <v>1.37004716239466</v>
+        <v>1.3700472171209785</v>
       </c>
       <c r="AA29" t="n">
-        <v>1.461436564230604</v>
+        <v>1.4614398540905496</v>
       </c>
       <c r="AB29" t="n">
-        <v>1.5412390633056794</v>
+        <v>1.5412542616925042</v>
       </c>
       <c r="AC29" t="n">
-        <v>1.6043817642068323</v>
+        <v>1.6044191931298108</v>
       </c>
       <c r="AD29" t="n">
-        <v>1.6490655998001533</v>
+        <v>1.6491327746270563</v>
       </c>
       <c r="AE29" t="n">
-        <v>1.6773250873440804</v>
+        <v>1.6774215958929224</v>
       </c>
       <c r="AF29" t="n">
-        <v>1.6949508399329367</v>
+        <v>1.6950661036778765</v>
       </c>
       <c r="AG29" t="n">
-        <v>1.7083726403498527</v>
+        <v>1.7084796707864247</v>
       </c>
       <c r="AH29" t="n">
-        <v>1.7287494041741325</v>
+        <v>1.7288007684789792</v>
       </c>
       <c r="AI29" t="n">
-        <v>1.770628858646468</v>
+        <v>1.7705525844000858</v>
       </c>
       <c r="AJ29" t="n">
-        <v>1.851545003830901</v>
+        <v>1.8512392306819614</v>
       </c>
     </row>
     <row r="30">
@@ -38207,40 +38207,40 @@
         <v>0.00668660898157837</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.006828743883997675</v>
+        <v>0.00682874388399651</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.006989984851111815</v>
+        <v>0.0069899847738513765</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.0071617817611837244</v>
+        <v>0.007161780076340141</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.007354212764990933</v>
+        <v>0.007354201328336692</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.007568168806684497</v>
+        <v>0.007568135458806586</v>
       </c>
       <c r="AD30" t="n">
-        <v>0.007814073546217598</v>
+        <v>0.007814005597324456</v>
       </c>
       <c r="AE30" t="n">
-        <v>0.008112094643072675</v>
+        <v>0.008111957197527503</v>
       </c>
       <c r="AF30" t="n">
-        <v>0.008507383537643277</v>
+        <v>0.008507191375901182</v>
       </c>
       <c r="AG30" t="n">
-        <v>0.008969519710505301</v>
+        <v>0.008969299096269458</v>
       </c>
       <c r="AH30" t="n">
-        <v>0.009492149536845696</v>
+        <v>0.009491964062900265</v>
       </c>
       <c r="AI30" t="n">
-        <v>0.010068615434911063</v>
+        <v>0.010068578644183286</v>
       </c>
       <c r="AJ30" t="n">
-        <v>0.01068224719870613</v>
+        <v>0.010682499821997503</v>
       </c>
     </row>
     <row r="31">
@@ -38317,40 +38317,40 @@
         <v>0.09150553148961957</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.1050207554479331</v>
+        <v>0.10502075544793288</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.11998006471626833</v>
+        <v>0.11998006470153162</v>
       </c>
       <c r="AA31" t="n">
-        <v>0.1362576096541747</v>
+        <v>0.1362576093328064</v>
       </c>
       <c r="AB31" t="n">
-        <v>0.1538248470049287</v>
+        <v>0.15382484482349285</v>
       </c>
       <c r="AC31" t="n">
-        <v>0.17280092766104146</v>
+        <v>0.17280092130024255</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.19325487713609507</v>
+        <v>0.1932548641754729</v>
       </c>
       <c r="AE31" t="n">
-        <v>0.21508731813249157</v>
+        <v>0.21508729191602657</v>
       </c>
       <c r="AF31" t="n">
-        <v>0.2382685972960791</v>
+        <v>0.2382685606430062</v>
       </c>
       <c r="AG31" t="n">
-        <v>0.26223348956529013</v>
+        <v>0.2622334474851675</v>
       </c>
       <c r="AH31" t="n">
-        <v>0.2784456170149448</v>
+        <v>0.27844558163750716</v>
       </c>
       <c r="AI31" t="n">
-        <v>0.28749417956466805</v>
+        <v>0.2874941725471774</v>
       </c>
       <c r="AJ31" t="n">
-        <v>0.29546402454049814</v>
+        <v>0.29546407272605174</v>
       </c>
     </row>
     <row r="32">
@@ -38427,40 +38427,40 @@
         <v>0.007728310686436527</v>
       </c>
       <c r="Y32" t="n">
-        <v>0.008107774406239188</v>
+        <v>0.008107774406236352</v>
       </c>
       <c r="Z32" t="n">
-        <v>0.008484177676904917</v>
+        <v>0.00848417750397023</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.008860354666972759</v>
+        <v>0.00886035114205525</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.009249627726981013</v>
+        <v>0.009249605171212122</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.009660938102349116</v>
+        <v>0.00966087670327678</v>
       </c>
       <c r="AD32" t="n">
-        <v>0.010101253140067044</v>
+        <v>0.010101134121542406</v>
       </c>
       <c r="AE32" t="n">
-        <v>0.010602005343085134</v>
+        <v>0.010601784694348733</v>
       </c>
       <c r="AF32" t="n">
-        <v>0.01121543234032172</v>
+        <v>0.011215150676482315</v>
       </c>
       <c r="AG32" t="n">
-        <v>0.011867354591149664</v>
+        <v>0.011867057852343717</v>
       </c>
       <c r="AH32" t="n">
-        <v>0.012549228791317871</v>
+        <v>0.012548994647192373</v>
       </c>
       <c r="AI32" t="n">
-        <v>0.013250319202694778</v>
+        <v>0.013250275400127035</v>
       </c>
       <c r="AJ32" t="n">
-        <v>0.013945675846396888</v>
+        <v>0.013945954453186651</v>
       </c>
     </row>
     <row r="33">
@@ -38547,40 +38547,40 @@
         <v>-0.03351875001416349</v>
       </c>
       <c r="Y35" t="n">
-        <v>-0.047482649857908676</v>
+        <v>-0.04748264985751277</v>
       </c>
       <c r="Z35" t="n">
-        <v>-0.061738528847355756</v>
+        <v>-0.06173850911064099</v>
       </c>
       <c r="AA35" t="n">
-        <v>-0.07638534498236965</v>
+        <v>-0.07638511601574477</v>
       </c>
       <c r="AB35" t="n">
-        <v>-0.0925083232187946</v>
+        <v>-0.09250649253915261</v>
       </c>
       <c r="AC35" t="n">
-        <v>-0.11059865190943985</v>
+        <v>-0.1105935523204718</v>
       </c>
       <c r="AD35" t="n">
-        <v>-0.13108792494711247</v>
+        <v>-0.13107794160828634</v>
       </c>
       <c r="AE35" t="n">
-        <v>-0.15816962325269684</v>
+        <v>-0.15814901378370866</v>
       </c>
       <c r="AF35" t="n">
-        <v>-0.19931138952287686</v>
+        <v>-0.1992849432102234</v>
       </c>
       <c r="AG35" t="n">
-        <v>-0.2450099278043017</v>
+        <v>-0.24498115649026636</v>
       </c>
       <c r="AH35" t="n">
-        <v>-0.2984628632388955</v>
+        <v>-0.29843658386743266</v>
       </c>
       <c r="AI35" t="n">
-        <v>-0.3606977760702632</v>
+        <v>-0.36068217145688686</v>
       </c>
       <c r="AJ35" t="n">
-        <v>-0.42937291586237636</v>
+        <v>-0.4293731952769524</v>
       </c>
     </row>
     <row r="36">
@@ -38672,40 +38672,40 @@
         <v>0.1080282442724167</v>
       </c>
       <c r="Y39" t="n">
-        <v>0.15014740640495844</v>
+        <v>0.1501474064046397</v>
       </c>
       <c r="Z39" t="n">
-        <v>0.1919268692548763</v>
+        <v>0.19192685005972226</v>
       </c>
       <c r="AA39" t="n">
-        <v>0.23368121574006323</v>
+        <v>0.2336808244863981</v>
       </c>
       <c r="AB39" t="n">
-        <v>0.27688918075142926</v>
+        <v>0.27688667713899645</v>
       </c>
       <c r="AC39" t="n">
-        <v>0.32254321164517125</v>
+        <v>0.3225363965602284</v>
       </c>
       <c r="AD39" t="n">
-        <v>0.37141665987015565</v>
+        <v>0.3714034492250425</v>
       </c>
       <c r="AE39" t="n">
-        <v>0.42699842467790144</v>
+        <v>0.42697393343034556</v>
       </c>
       <c r="AF39" t="n">
-        <v>0.4950867024361027</v>
+        <v>0.495055438722874</v>
       </c>
       <c r="AG39" t="n">
-        <v>0.5674478203704165</v>
+        <v>0.5674148833879689</v>
       </c>
       <c r="AH39" t="n">
-        <v>0.6431335012197412</v>
+        <v>0.6431075120306031</v>
       </c>
       <c r="AI39" t="n">
-        <v>0.7209522721993691</v>
+        <v>0.7209474099305384</v>
       </c>
       <c r="AJ39" t="n">
-        <v>0.7983734486798666</v>
+        <v>0.7984046091545502</v>
       </c>
     </row>
     <row r="40">
@@ -38782,40 +38782,40 @@
         <v>1.1455631620100106</v>
       </c>
       <c r="Y40" t="n">
-        <v>1.240969750816219</v>
+        <v>1.2409697508161581</v>
       </c>
       <c r="Z40" t="n">
-        <v>1.3362450859429378</v>
+        <v>1.3362451406692566</v>
       </c>
       <c r="AA40" t="n">
-        <v>1.427634487778882</v>
+        <v>1.4276377776388276</v>
       </c>
       <c r="AB40" t="n">
-        <v>1.5074369868539574</v>
+        <v>1.5074521852407823</v>
       </c>
       <c r="AC40" t="n">
-        <v>1.5705796877551101</v>
+        <v>1.5706171166780887</v>
       </c>
       <c r="AD40" t="n">
-        <v>1.6152635233484314</v>
+        <v>1.6153306981753344</v>
       </c>
       <c r="AE40" t="n">
-        <v>1.6435230108923584</v>
+        <v>1.6436195194412004</v>
       </c>
       <c r="AF40" t="n">
-        <v>1.6611487634812148</v>
+        <v>1.6612640272261543</v>
       </c>
       <c r="AG40" t="n">
-        <v>1.6745705638981307</v>
+        <v>1.6746775943347025</v>
       </c>
       <c r="AH40" t="n">
-        <v>1.6949234354533254</v>
+        <v>1.694974828410584</v>
       </c>
       <c r="AI40" t="n">
-        <v>1.7366116329574885</v>
+        <v>1.7365353922718616</v>
       </c>
       <c r="AJ40" t="n">
-        <v>1.8170995877575402</v>
+        <v>1.8167936371147129</v>
       </c>
     </row>
     <row r="41">
@@ -38892,40 +38892,40 @@
         <v>0.00784660898157837</v>
       </c>
       <c r="Y41" t="n">
-        <v>0.007988743883997675</v>
+        <v>0.00798874388399651</v>
       </c>
       <c r="Z41" t="n">
-        <v>0.008149984851111815</v>
+        <v>0.008149984773851376</v>
       </c>
       <c r="AA41" t="n">
-        <v>0.008321781761183724</v>
+        <v>0.008321780076340142</v>
       </c>
       <c r="AB41" t="n">
-        <v>0.008514212764990934</v>
+        <v>0.008514201328336692</v>
       </c>
       <c r="AC41" t="n">
-        <v>0.008728168806684497</v>
+        <v>0.008728135458806586</v>
       </c>
       <c r="AD41" t="n">
-        <v>0.008974073546217598</v>
+        <v>0.008974005597324457</v>
       </c>
       <c r="AE41" t="n">
-        <v>0.009272094643072677</v>
+        <v>0.009271957197527502</v>
       </c>
       <c r="AF41" t="n">
-        <v>0.009667383537643277</v>
+        <v>0.009667191375901182</v>
       </c>
       <c r="AG41" t="n">
-        <v>0.0101295197105053</v>
+        <v>0.010129299096269457</v>
       </c>
       <c r="AH41" t="n">
-        <v>0.010652149536845696</v>
+        <v>0.010651964062900265</v>
       </c>
       <c r="AI41" t="n">
-        <v>0.011228615434911063</v>
+        <v>0.011228578644183286</v>
       </c>
       <c r="AJ41" t="n">
-        <v>0.01184224719870613</v>
+        <v>0.011842499821997502</v>
       </c>
     </row>
     <row r="42">
@@ -39002,40 +39002,40 @@
         <v>0.09172679074819215</v>
       </c>
       <c r="Y42" t="n">
-        <v>0.1052420147065057</v>
+        <v>0.10524201470650547</v>
       </c>
       <c r="Z42" t="n">
-        <v>0.12020132397484092</v>
+        <v>0.1202013239601042</v>
       </c>
       <c r="AA42" t="n">
-        <v>0.1364788689127473</v>
+        <v>0.13647886859137898</v>
       </c>
       <c r="AB42" t="n">
-        <v>0.15404610626350135</v>
+        <v>0.15404610408206543</v>
       </c>
       <c r="AC42" t="n">
-        <v>0.17302218691961405</v>
+        <v>0.17302218055881513</v>
       </c>
       <c r="AD42" t="n">
-        <v>0.19347613639466768</v>
+        <v>0.1934761234340455</v>
       </c>
       <c r="AE42" t="n">
-        <v>0.21530857739106415</v>
+        <v>0.21530855117459916</v>
       </c>
       <c r="AF42" t="n">
-        <v>0.23848985655465169</v>
+        <v>0.23848981990157878</v>
       </c>
       <c r="AG42" t="n">
-        <v>0.26245474882386277</v>
+        <v>0.26245470674374016</v>
       </c>
       <c r="AH42" t="n">
-        <v>0.2786668762735174</v>
+        <v>0.27866684089607974</v>
       </c>
       <c r="AI42" t="n">
-        <v>0.28771543882324063</v>
+        <v>0.28771543180575</v>
       </c>
       <c r="AJ42" t="n">
-        <v>0.2956852837990707</v>
+        <v>0.2956853319846243</v>
       </c>
     </row>
     <row r="43">
@@ -39112,40 +39112,40 @@
         <v>0.01748691011846544</v>
       </c>
       <c r="Y43" t="n">
-        <v>0.017866373838268102</v>
+        <v>0.017866373838265268</v>
       </c>
       <c r="Z43" t="n">
-        <v>0.018242777108933832</v>
+        <v>0.018242776935999145</v>
       </c>
       <c r="AA43" t="n">
-        <v>0.018618954099001675</v>
+        <v>0.018618950574084164</v>
       </c>
       <c r="AB43" t="n">
-        <v>0.01900822715900993</v>
+        <v>0.019008204603241034</v>
       </c>
       <c r="AC43" t="n">
-        <v>0.019419537534378032</v>
+        <v>0.019419476135305695</v>
       </c>
       <c r="AD43" t="n">
-        <v>0.019859852572095958</v>
+        <v>0.01985973355357132</v>
       </c>
       <c r="AE43" t="n">
-        <v>0.02036060477511405</v>
+        <v>0.020360384126377647</v>
       </c>
       <c r="AF43" t="n">
-        <v>0.020974031772350635</v>
+        <v>0.02097375010851123</v>
       </c>
       <c r="AG43" t="n">
-        <v>0.02162595402317858</v>
+        <v>0.02162565728437263</v>
       </c>
       <c r="AH43" t="n">
-        <v>0.022307828223346787</v>
+        <v>0.02230759407922129</v>
       </c>
       <c r="AI43" t="n">
-        <v>0.023008918634723693</v>
+        <v>0.02300887483215595</v>
       </c>
       <c r="AJ43" t="n">
-        <v>0.023704275278425804</v>
+        <v>0.023704553885215567</v>
       </c>
     </row>
     <row r="44">
@@ -39232,40 +39232,40 @@
         <v>0.18785428493157047</v>
       </c>
       <c r="Y46" t="n">
-        <v>0.17446381417955734</v>
+        <v>0.1744638141799531</v>
       </c>
       <c r="Z46" t="n">
-        <v>0.16072582575217645</v>
+        <v>0.16072584548889113</v>
       </c>
       <c r="AA46" t="n">
-        <v>0.1465412312733831</v>
+        <v>0.14654146024000808</v>
       </c>
       <c r="AB46" t="n">
-        <v>0.13082468942550377</v>
+        <v>0.13082652010514573</v>
       </c>
       <c r="AC46" t="n">
-        <v>0.11308490953754113</v>
+        <v>0.11309000912650932</v>
       </c>
       <c r="AD46" t="n">
-        <v>0.09289020946790211</v>
+        <v>0.09290019280672812</v>
       </c>
       <c r="AE46" t="n">
-        <v>0.06604703413853275</v>
+        <v>0.0660676436075211</v>
       </c>
       <c r="AF46" t="n">
-        <v>0.025087680805865542</v>
+        <v>0.025114127118519125</v>
       </c>
       <c r="AG46" t="n">
-        <v>-0.020484600498230365</v>
+        <v>-0.020455829184194863</v>
       </c>
       <c r="AH46" t="n">
-        <v>-0.07370967672892736</v>
+        <v>-0.07368358658450036</v>
       </c>
       <c r="AI46" t="n">
-        <v>-0.13466738542674306</v>
+        <v>-0.13465200249300402</v>
       </c>
       <c r="AJ46" t="n">
-        <v>-0.2005568989482226</v>
+        <v>-0.2005560060588878</v>
       </c>
     </row>
     <row r="47">
@@ -39357,40 +39357,40 @@
         <v>-0.03803039260768415</v>
       </c>
       <c r="Y50" t="n">
-        <v>0.004088769524857594</v>
+        <v>0.004088769524538849</v>
       </c>
       <c r="Z50" t="n">
-        <v>0.04586823237477544</v>
+        <v>0.04586821317962142</v>
       </c>
       <c r="AA50" t="n">
-        <v>0.08762257885996239</v>
+        <v>0.08762218760629725</v>
       </c>
       <c r="AB50" t="n">
-        <v>0.13083054387132842</v>
+        <v>0.1308280402588956</v>
       </c>
       <c r="AC50" t="n">
-        <v>0.1764845747650704</v>
+        <v>0.17647775968012758</v>
       </c>
       <c r="AD50" t="n">
-        <v>0.2253580229900548</v>
+        <v>0.22534481234494164</v>
       </c>
       <c r="AE50" t="n">
-        <v>0.2809397877978006</v>
+        <v>0.2809152965502447</v>
       </c>
       <c r="AF50" t="n">
-        <v>0.34902806555600185</v>
+        <v>0.34899680184277315</v>
       </c>
       <c r="AG50" t="n">
-        <v>0.4213891834903156</v>
+        <v>0.42135624650786796</v>
       </c>
       <c r="AH50" t="n">
-        <v>0.49707486433964043</v>
+        <v>0.49704887515050233</v>
       </c>
       <c r="AI50" t="n">
-        <v>0.5748934782553662</v>
+        <v>0.5748886163216559</v>
       </c>
       <c r="AJ50" t="n">
-        <v>0.6520756637651145</v>
+        <v>0.652106588156408</v>
       </c>
     </row>
     <row r="51">
@@ -39467,40 +39467,40 @@
         <v>1.117703829506378</v>
       </c>
       <c r="Y51" t="n">
-        <v>1.2131104183125863</v>
+        <v>1.2131104183125254</v>
       </c>
       <c r="Z51" t="n">
-        <v>1.308385753439305</v>
+        <v>1.3083858081656237</v>
       </c>
       <c r="AA51" t="n">
-        <v>1.399775155275249</v>
+        <v>1.399778445135195</v>
       </c>
       <c r="AB51" t="n">
-        <v>1.4795776543503247</v>
+        <v>1.4795928527371496</v>
       </c>
       <c r="AC51" t="n">
-        <v>1.5427203552514774</v>
+        <v>1.542757784174456</v>
       </c>
       <c r="AD51" t="n">
-        <v>1.5874041908447987</v>
+        <v>1.5874713656717017</v>
       </c>
       <c r="AE51" t="n">
-        <v>1.6156636783887257</v>
+        <v>1.6157601869375675</v>
       </c>
       <c r="AF51" t="n">
-        <v>1.633289430977582</v>
+        <v>1.6334046947225216</v>
       </c>
       <c r="AG51" t="n">
-        <v>1.6467112313944978</v>
+        <v>1.6468182618310698</v>
       </c>
       <c r="AH51" t="n">
-        <v>1.6670641029496926</v>
+        <v>1.6671154959069512</v>
       </c>
       <c r="AI51" t="n">
-        <v>1.708752270495371</v>
+        <v>1.708676029873665</v>
       </c>
       <c r="AJ51" t="n">
-        <v>1.789194639980773</v>
+        <v>1.7888886443072252</v>
       </c>
     </row>
     <row r="52">
@@ -39577,40 +39577,40 @@
         <v>0.00978660898157837</v>
       </c>
       <c r="Y52" t="n">
-        <v>0.009928743883997676</v>
+        <v>0.00992874388399651</v>
       </c>
       <c r="Z52" t="n">
-        <v>0.010089984851111814</v>
+        <v>0.010089984773851377</v>
       </c>
       <c r="AA52" t="n">
-        <v>0.010261781761183725</v>
+        <v>0.01026178007634014</v>
       </c>
       <c r="AB52" t="n">
-        <v>0.010454212764990933</v>
+        <v>0.010454201328336693</v>
       </c>
       <c r="AC52" t="n">
-        <v>0.010668168806684497</v>
+        <v>0.010668135458806585</v>
       </c>
       <c r="AD52" t="n">
-        <v>0.010914073546217599</v>
+        <v>0.010914005597324456</v>
       </c>
       <c r="AE52" t="n">
-        <v>0.011212094643072676</v>
+        <v>0.011211957197527503</v>
       </c>
       <c r="AF52" t="n">
-        <v>0.011607383537643278</v>
+        <v>0.011607191375901183</v>
       </c>
       <c r="AG52" t="n">
-        <v>0.012069519710505301</v>
+        <v>0.012069299096269458</v>
       </c>
       <c r="AH52" t="n">
-        <v>0.012592149536845697</v>
+        <v>0.012591964062900265</v>
       </c>
       <c r="AI52" t="n">
-        <v>0.013168615434911064</v>
+        <v>0.013168578644183287</v>
       </c>
       <c r="AJ52" t="n">
-        <v>0.01378224719870613</v>
+        <v>0.013782499821997503</v>
       </c>
     </row>
     <row r="53">
@@ -39687,40 +39687,40 @@
         <v>0.09209682778408079</v>
       </c>
       <c r="Y53" t="n">
-        <v>0.10561205174239434</v>
+        <v>0.1056120517423941</v>
       </c>
       <c r="Z53" t="n">
-        <v>0.12057136101072956</v>
+        <v>0.12057136099599285</v>
       </c>
       <c r="AA53" t="n">
-        <v>0.13684890594863594</v>
+        <v>0.13684890562726762</v>
       </c>
       <c r="AB53" t="n">
-        <v>0.15441614329938996</v>
+        <v>0.15441614111795404</v>
       </c>
       <c r="AC53" t="n">
-        <v>0.1733922239555027</v>
+        <v>0.17339221759470377</v>
       </c>
       <c r="AD53" t="n">
-        <v>0.1938461734305563</v>
+        <v>0.19384616046993414</v>
       </c>
       <c r="AE53" t="n">
-        <v>0.21567861442695282</v>
+        <v>0.21567858821048777</v>
       </c>
       <c r="AF53" t="n">
-        <v>0.23885989359054036</v>
+        <v>0.23885985693746745</v>
       </c>
       <c r="AG53" t="n">
-        <v>0.26282478585975144</v>
+        <v>0.2628247437796288</v>
       </c>
       <c r="AH53" t="n">
-        <v>0.279036913309406</v>
+        <v>0.27903687793196835</v>
       </c>
       <c r="AI53" t="n">
-        <v>0.2880854758591293</v>
+        <v>0.2880854688416386</v>
       </c>
       <c r="AJ53" t="n">
-        <v>0.2960553208349594</v>
+        <v>0.29605536902051294</v>
       </c>
     </row>
     <row r="54">
@@ -39797,40 +39797,40 @@
         <v>0.030060640420565197</v>
       </c>
       <c r="Y54" t="n">
-        <v>0.03044010414036786</v>
+        <v>0.03044010414036502</v>
       </c>
       <c r="Z54" t="n">
-        <v>0.03081650741103359</v>
+        <v>0.0308165072380989</v>
       </c>
       <c r="AA54" t="n">
-        <v>0.031192684401101428</v>
+        <v>0.03119268087618392</v>
       </c>
       <c r="AB54" t="n">
-        <v>0.031581957461109686</v>
+        <v>0.031581934905340794</v>
       </c>
       <c r="AC54" t="n">
-        <v>0.03199326783647779</v>
+        <v>0.03199320643740545</v>
       </c>
       <c r="AD54" t="n">
-        <v>0.03243358287419571</v>
+        <v>0.03243346385567108</v>
       </c>
       <c r="AE54" t="n">
-        <v>0.03293433507721381</v>
+        <v>0.0329341144284774</v>
       </c>
       <c r="AF54" t="n">
-        <v>0.03354776207445039</v>
+        <v>0.03354748041061099</v>
       </c>
       <c r="AG54" t="n">
-        <v>0.03419968432527833</v>
+        <v>0.03419938758647238</v>
       </c>
       <c r="AH54" t="n">
-        <v>0.03488155852544654</v>
+        <v>0.03488132438132104</v>
       </c>
       <c r="AI54" t="n">
-        <v>0.03558264893682345</v>
+        <v>0.03558260513425571</v>
       </c>
       <c r="AJ54" t="n">
-        <v>0.03627800558052556</v>
+        <v>0.036278284187315324</v>
       </c>
     </row>
     <row r="55">
@@ -39917,40 +39917,40 @@
         <v>0.3711444674940651</v>
       </c>
       <c r="Y57" t="n">
-        <v>0.3582072226470388</v>
+        <v>0.3582072226474346</v>
       </c>
       <c r="Z57" t="n">
-        <v>0.3448766357378914</v>
+        <v>0.3448766554746061</v>
       </c>
       <c r="AA57" t="n">
-        <v>0.3310535158294246</v>
+        <v>0.33105374479604965</v>
       </c>
       <c r="AB57" t="n">
-        <v>0.31565243060467485</v>
+        <v>0.31565426128431695</v>
       </c>
       <c r="AC57" t="n">
-        <v>0.29818200997812705</v>
+        <v>0.29818710956709527</v>
       </c>
       <c r="AD57" t="n">
-        <v>0.27821050399843444</v>
+        <v>0.27822048733726046</v>
       </c>
       <c r="AE57" t="n">
-        <v>0.2515443013996244</v>
+        <v>0.25156491086861266</v>
       </c>
       <c r="AF57" t="n">
-        <v>0.21071565488619098</v>
+        <v>0.21074210119884462</v>
       </c>
       <c r="AG57" t="n">
-        <v>0.1652277815852609</v>
+        <v>0.16525655289929642</v>
       </c>
       <c r="AH57" t="n">
-        <v>0.11204079329239763</v>
+        <v>0.1120668834368247</v>
       </c>
       <c r="AI57" t="n">
-        <v>0.05107504076412672</v>
+        <v>0.051090423275645835</v>
       </c>
       <c r="AJ57" t="n">
-        <v>-0.014567962165603299</v>
+        <v>-0.014566771859323868</v>
       </c>
     </row>
     <row r="58">
@@ -40042,40 +40042,40 @@
         <v>-0.061440853437131904</v>
       </c>
       <c r="Y61" t="n">
-        <v>-0.01932169130459016</v>
+        <v>-0.019321691304908906</v>
       </c>
       <c r="Z61" t="n">
-        <v>0.022457771545327687</v>
+        <v>0.022457752350173665</v>
       </c>
       <c r="AA61" t="n">
-        <v>0.06421211803051463</v>
+        <v>0.0642117267768495</v>
       </c>
       <c r="AB61" t="n">
-        <v>0.10742008304188067</v>
+        <v>0.10741757942944785</v>
       </c>
       <c r="AC61" t="n">
-        <v>0.15307411393562265</v>
+        <v>0.15306729885067982</v>
       </c>
       <c r="AD61" t="n">
-        <v>0.20194756216060705</v>
+        <v>0.20193435151549388</v>
       </c>
       <c r="AE61" t="n">
-        <v>0.25752932696835285</v>
+        <v>0.25750483572079697</v>
       </c>
       <c r="AF61" t="n">
-        <v>0.3256176047265541</v>
+        <v>0.3255863410133254</v>
       </c>
       <c r="AG61" t="n">
-        <v>0.39797872266086787</v>
+        <v>0.3979457856784202</v>
       </c>
       <c r="AH61" t="n">
-        <v>0.4736644035101927</v>
+        <v>0.4736384143210546</v>
       </c>
       <c r="AI61" t="n">
-        <v>0.5514830174259184</v>
+        <v>0.5514781554922081</v>
       </c>
       <c r="AJ61" t="n">
-        <v>0.6286833451053826</v>
+        <v>0.6287143155263288</v>
       </c>
     </row>
     <row r="62">
@@ -40152,40 +40152,40 @@
         <v>1.113238500880545</v>
       </c>
       <c r="Y62" t="n">
-        <v>1.2086450896867533</v>
+        <v>1.2086450896866925</v>
       </c>
       <c r="Z62" t="n">
-        <v>1.3039204248134721</v>
+        <v>1.3039204795397907</v>
       </c>
       <c r="AA62" t="n">
-        <v>1.3953098266494162</v>
+        <v>1.395313116509362</v>
       </c>
       <c r="AB62" t="n">
-        <v>1.4751123257244918</v>
+        <v>1.4751275241113164</v>
       </c>
       <c r="AC62" t="n">
-        <v>1.5382550266256445</v>
+        <v>1.538292455548623</v>
       </c>
       <c r="AD62" t="n">
-        <v>1.5829388622189657</v>
+        <v>1.5830060370458687</v>
       </c>
       <c r="AE62" t="n">
-        <v>1.6111983497628928</v>
+        <v>1.6112948583117346</v>
       </c>
       <c r="AF62" t="n">
-        <v>1.628824102351749</v>
+        <v>1.6289393660966887</v>
       </c>
       <c r="AG62" t="n">
-        <v>1.642245902768665</v>
+        <v>1.642352933205237</v>
       </c>
       <c r="AH62" t="n">
-        <v>1.6625987743238595</v>
+        <v>1.662650167281118</v>
       </c>
       <c r="AI62" t="n">
-        <v>1.704286941869538</v>
+        <v>1.704210701247832</v>
       </c>
       <c r="AJ62" t="n">
-        <v>1.7847327718058197</v>
+        <v>1.7844267849120017</v>
       </c>
     </row>
     <row r="63">
@@ -40262,40 +40262,40 @@
         <v>0.01250660898157837</v>
       </c>
       <c r="Y63" t="n">
-        <v>0.012648743883997674</v>
+        <v>0.012648743883996508</v>
       </c>
       <c r="Z63" t="n">
-        <v>0.012809984851111815</v>
+        <v>0.012809984773851375</v>
       </c>
       <c r="AA63" t="n">
-        <v>0.012981781761183725</v>
+        <v>0.01298178007634014</v>
       </c>
       <c r="AB63" t="n">
-        <v>0.013174212764990933</v>
+        <v>0.013174201328336691</v>
       </c>
       <c r="AC63" t="n">
-        <v>0.013388168806684496</v>
+        <v>0.013388135458806585</v>
       </c>
       <c r="AD63" t="n">
-        <v>0.013634073546217599</v>
+        <v>0.013634005597324457</v>
       </c>
       <c r="AE63" t="n">
-        <v>0.013932094643072676</v>
+        <v>0.013931957197527503</v>
       </c>
       <c r="AF63" t="n">
-        <v>0.014327383537643276</v>
+        <v>0.014327191375901181</v>
       </c>
       <c r="AG63" t="n">
-        <v>0.014789519710505301</v>
+        <v>0.014789299096269456</v>
       </c>
       <c r="AH63" t="n">
-        <v>0.015312149536845697</v>
+        <v>0.015311964062900266</v>
       </c>
       <c r="AI63" t="n">
-        <v>0.015888615434911064</v>
+        <v>0.015888578644183287</v>
       </c>
       <c r="AJ63" t="n">
-        <v>0.01650224719870613</v>
+        <v>0.0165024998219975</v>
       </c>
     </row>
     <row r="64">
@@ -40372,40 +40372,40 @@
         <v>0.09261564259728548</v>
       </c>
       <c r="Y64" t="n">
-        <v>0.10613086655559902</v>
+        <v>0.1061308665555988</v>
       </c>
       <c r="Z64" t="n">
-        <v>0.12109017582393425</v>
+        <v>0.12109017580919754</v>
       </c>
       <c r="AA64" t="n">
-        <v>0.13736772076184062</v>
+        <v>0.1373677204404723</v>
       </c>
       <c r="AB64" t="n">
-        <v>0.15493495811259467</v>
+        <v>0.15493495593115875</v>
       </c>
       <c r="AC64" t="n">
-        <v>0.17391103876870737</v>
+        <v>0.17391103240790845</v>
       </c>
       <c r="AD64" t="n">
-        <v>0.194364988243761</v>
+        <v>0.19436497528313884</v>
       </c>
       <c r="AE64" t="n">
-        <v>0.21619742924015747</v>
+        <v>0.21619740302369247</v>
       </c>
       <c r="AF64" t="n">
-        <v>0.23937870840374506</v>
+        <v>0.23937867175067215</v>
       </c>
       <c r="AG64" t="n">
-        <v>0.2633436006729561</v>
+        <v>0.2633435585928334</v>
       </c>
       <c r="AH64" t="n">
-        <v>0.2795557281226107</v>
+        <v>0.27955569274517306</v>
       </c>
       <c r="AI64" t="n">
-        <v>0.28860429067233395</v>
+        <v>0.2886042836548433</v>
       </c>
       <c r="AJ64" t="n">
-        <v>0.29657413564816404</v>
+        <v>0.29657418383371764</v>
       </c>
     </row>
     <row r="65">
@@ -40482,40 +40482,40 @@
         <v>0.04474492828537198</v>
       </c>
       <c r="Y65" t="n">
-        <v>0.04512439200517464</v>
+        <v>0.0451243920051718</v>
       </c>
       <c r="Z65" t="n">
-        <v>0.04550079527584037</v>
+        <v>0.04550079510290568</v>
       </c>
       <c r="AA65" t="n">
-        <v>0.04587697226590821</v>
+        <v>0.045876968740990696</v>
       </c>
       <c r="AB65" t="n">
-        <v>0.046266245325916465</v>
+        <v>0.046266222770147566</v>
       </c>
       <c r="AC65" t="n">
-        <v>0.04667755570128457</v>
+        <v>0.04667749430221223</v>
       </c>
       <c r="AD65" t="n">
-        <v>0.04711787073900249</v>
+        <v>0.04711775172047786</v>
       </c>
       <c r="AE65" t="n">
-        <v>0.047618622942020586</v>
+        <v>0.04761840229328418</v>
       </c>
       <c r="AF65" t="n">
-        <v>0.04823204993925717</v>
+        <v>0.048231768275417766</v>
       </c>
       <c r="AG65" t="n">
-        <v>0.04888397219008511</v>
+        <v>0.04888367545127917</v>
       </c>
       <c r="AH65" t="n">
-        <v>0.04956584639025332</v>
+        <v>0.04956561224612782</v>
       </c>
       <c r="AI65" t="n">
-        <v>0.050266936801630226</v>
+        <v>0.050266892999062486</v>
       </c>
       <c r="AJ65" t="n">
-        <v>0.05096229344533234</v>
+        <v>0.0509625720521221</v>
       </c>
     </row>
     <row r="66">
@@ -40602,40 +40602,40 @@
         <v>0.4027862051231064</v>
       </c>
       <c r="Y68" t="n">
-        <v>0.389874133296092</v>
+        <v>0.3898741332964878</v>
       </c>
       <c r="Z68" t="n">
-        <v>0.376561251984077</v>
+        <v>0.3765612717207917</v>
       </c>
       <c r="AA68" t="n">
-        <v>0.3627483657925735</v>
+        <v>0.3627485947591985</v>
       </c>
       <c r="AB68" t="n">
-        <v>0.3473500398283347</v>
+        <v>0.34735187050797667</v>
       </c>
       <c r="AC68" t="n">
-        <v>0.32987490331121616</v>
+        <v>0.32988000290018427</v>
       </c>
       <c r="AD68" t="n">
-        <v>0.30989120747707155</v>
+        <v>0.3099011908158976</v>
       </c>
       <c r="AE68" t="n">
-        <v>0.28320534412865883</v>
+        <v>0.2832259535976471</v>
       </c>
       <c r="AF68" t="n">
-        <v>0.24234957091996073</v>
+        <v>0.24237601723261437</v>
       </c>
       <c r="AG68" t="n">
-        <v>0.19682711180710416</v>
+        <v>0.19685588312113966</v>
       </c>
       <c r="AH68" t="n">
-        <v>0.1435980872924461</v>
+        <v>0.14362417743687317</v>
       </c>
       <c r="AI68" t="n">
-        <v>0.082582858714906</v>
+        <v>0.08259824122642523</v>
       </c>
       <c r="AJ68" t="n">
-        <v>0.016860096928294765</v>
+        <v>0.016861229246595055</v>
       </c>
     </row>
     <row r="69">
@@ -40727,40 +40727,40 @@
         <v>-0.09540356519722093</v>
       </c>
       <c r="Y72" t="n">
-        <v>-0.05328440306467919</v>
+        <v>-0.05328440306499793</v>
       </c>
       <c r="Z72" t="n">
-        <v>-0.011504940214761339</v>
+        <v>-0.01150495940991536</v>
       </c>
       <c r="AA72" t="n">
-        <v>0.030249406270425605</v>
+        <v>0.030249015016760472</v>
       </c>
       <c r="AB72" t="n">
-        <v>0.07345737128179164</v>
+        <v>0.07345486766935883</v>
       </c>
       <c r="AC72" t="n">
-        <v>0.11911140217553362</v>
+        <v>0.1191045870905908</v>
       </c>
       <c r="AD72" t="n">
-        <v>0.16798485040051803</v>
+        <v>0.16797163975540486</v>
       </c>
       <c r="AE72" t="n">
-        <v>0.22356661520826382</v>
+        <v>0.22354212396070794</v>
       </c>
       <c r="AF72" t="n">
-        <v>0.2916548929664651</v>
+        <v>0.29162362925323637</v>
       </c>
       <c r="AG72" t="n">
-        <v>0.36401601090077884</v>
+        <v>0.3639830739183312</v>
       </c>
       <c r="AH72" t="n">
-        <v>0.43970169175010365</v>
+        <v>0.43967570256096555</v>
       </c>
       <c r="AI72" t="n">
-        <v>0.5175203056658294</v>
+        <v>0.5175154437321191</v>
       </c>
       <c r="AJ72" t="n">
-        <v>0.5948680723433903</v>
+        <v>0.5948991846660789</v>
       </c>
     </row>
     <row r="73">
@@ -40837,40 +40837,40 @@
         <v>1.1067604281019658</v>
       </c>
       <c r="Y73" t="n">
-        <v>1.2021670169081742</v>
+        <v>1.2021670169081133</v>
       </c>
       <c r="Z73" t="n">
-        <v>1.297442352034893</v>
+        <v>1.2974424067612116</v>
       </c>
       <c r="AA73" t="n">
-        <v>1.388831753870837</v>
+        <v>1.3888350437307828</v>
       </c>
       <c r="AB73" t="n">
-        <v>1.4686342529459127</v>
+        <v>1.4686494513327373</v>
       </c>
       <c r="AC73" t="n">
-        <v>1.5317769538470654</v>
+        <v>1.531814382770044</v>
       </c>
       <c r="AD73" t="n">
-        <v>1.5764607894403866</v>
+        <v>1.5765279642672896</v>
       </c>
       <c r="AE73" t="n">
-        <v>1.6047202769843136</v>
+        <v>1.6048167855331554</v>
       </c>
       <c r="AF73" t="n">
-        <v>1.6223460295731698</v>
+        <v>1.6224612933181095</v>
       </c>
       <c r="AG73" t="n">
-        <v>1.6357678299900857</v>
+        <v>1.6358748604266578</v>
       </c>
       <c r="AH73" t="n">
-        <v>1.6561207015452803</v>
+        <v>1.6561720945025389</v>
       </c>
       <c r="AI73" t="n">
-        <v>1.6978088690909587</v>
+        <v>1.6977326284692529</v>
       </c>
       <c r="AJ73" t="n">
-        <v>1.7782828216508642</v>
+        <v>1.7779768618234897</v>
       </c>
     </row>
     <row r="74">
@@ -40947,40 +40947,40 @@
         <v>0.01600660898157837</v>
       </c>
       <c r="Y74" t="n">
-        <v>0.016148743883997674</v>
+        <v>0.016148743883996508</v>
       </c>
       <c r="Z74" t="n">
-        <v>0.016309984851111816</v>
+        <v>0.01630998477385138</v>
       </c>
       <c r="AA74" t="n">
-        <v>0.016481781761183725</v>
+        <v>0.01648178007634014</v>
       </c>
       <c r="AB74" t="n">
-        <v>0.016674212764990932</v>
+        <v>0.01667420132833669</v>
       </c>
       <c r="AC74" t="n">
-        <v>0.0168881688066845</v>
+        <v>0.016888135458806585</v>
       </c>
       <c r="AD74" t="n">
-        <v>0.0171340735462176</v>
+        <v>0.017134005597324458</v>
       </c>
       <c r="AE74" t="n">
-        <v>0.017432094643072677</v>
+        <v>0.017431957197527503</v>
       </c>
       <c r="AF74" t="n">
-        <v>0.01782738353764328</v>
+        <v>0.017827191375901184</v>
       </c>
       <c r="AG74" t="n">
-        <v>0.0182895197105053</v>
+        <v>0.01828929909626946</v>
       </c>
       <c r="AH74" t="n">
-        <v>0.018812149536845697</v>
+        <v>0.018811964062900265</v>
       </c>
       <c r="AI74" t="n">
-        <v>0.019388615434911063</v>
+        <v>0.019388578644183287</v>
       </c>
       <c r="AJ74" t="n">
-        <v>0.02000224719870613</v>
+        <v>0.020002499821997505</v>
       </c>
     </row>
     <row r="75">
@@ -41057,40 +41057,40 @@
         <v>0.09328323518780622</v>
       </c>
       <c r="Y75" t="n">
-        <v>0.10679845914611977</v>
+        <v>0.10679845914611955</v>
       </c>
       <c r="Z75" t="n">
-        <v>0.12175776841445499</v>
+        <v>0.12175776839971827</v>
       </c>
       <c r="AA75" t="n">
-        <v>0.13803531335236136</v>
+        <v>0.13803531303099303</v>
       </c>
       <c r="AB75" t="n">
-        <v>0.1556025507031154</v>
+        <v>0.15560254852167948</v>
       </c>
       <c r="AC75" t="n">
-        <v>0.1745786313592281</v>
+        <v>0.1745786249984292</v>
       </c>
       <c r="AD75" t="n">
-        <v>0.19503258083428174</v>
+        <v>0.19503256787365958</v>
       </c>
       <c r="AE75" t="n">
-        <v>0.2168650218306782</v>
+        <v>0.2168649956142132</v>
       </c>
       <c r="AF75" t="n">
-        <v>0.2400463009942658</v>
+        <v>0.2400462643411929</v>
       </c>
       <c r="AG75" t="n">
-        <v>0.26401119326347683</v>
+        <v>0.26401115118335416</v>
       </c>
       <c r="AH75" t="n">
-        <v>0.28022332071313144</v>
+        <v>0.2802232853356938</v>
       </c>
       <c r="AI75" t="n">
-        <v>0.2892718832628547</v>
+        <v>0.28927187624536405</v>
       </c>
       <c r="AJ75" t="n">
-        <v>0.29724172823868483</v>
+        <v>0.2972417764242384</v>
       </c>
     </row>
     <row r="76">
@@ -41167,40 +41167,40 @@
         <v>0.060224517314339934</v>
       </c>
       <c r="Y76" t="n">
-        <v>0.0606039810341426</v>
+        <v>0.06060398103413976</v>
       </c>
       <c r="Z76" t="n">
-        <v>0.06098038430480833</v>
+        <v>0.06098038413187364</v>
       </c>
       <c r="AA76" t="n">
-        <v>0.06135656129487617</v>
+        <v>0.06135655776995866</v>
       </c>
       <c r="AB76" t="n">
-        <v>0.06174583435488443</v>
+        <v>0.061745811799115535</v>
       </c>
       <c r="AC76" t="n">
-        <v>0.06215714473025253</v>
+        <v>0.06215708333118019</v>
       </c>
       <c r="AD76" t="n">
-        <v>0.06259745976797046</v>
+        <v>0.06259734074944581</v>
       </c>
       <c r="AE76" t="n">
-        <v>0.06309821197098854</v>
+        <v>0.06309799132225215</v>
       </c>
       <c r="AF76" t="n">
-        <v>0.06371163896822513</v>
+        <v>0.06371135730438572</v>
       </c>
       <c r="AG76" t="n">
-        <v>0.06436356121905307</v>
+        <v>0.06436326448024712</v>
       </c>
       <c r="AH76" t="n">
-        <v>0.06504543541922128</v>
+        <v>0.06504520127509579</v>
       </c>
       <c r="AI76" t="n">
-        <v>0.06574652583059819</v>
+        <v>0.06574648202803045</v>
       </c>
       <c r="AJ76" t="n">
-        <v>0.0664418824743003</v>
+        <v>0.06644216108109006</v>
       </c>
     </row>
     <row r="77">
@@ -41287,40 +41287,40 @@
         <v>0.4477966008270274</v>
       </c>
       <c r="Y79" t="n">
-        <v>0.4349298379618572</v>
+        <v>0.43492983796225293</v>
       </c>
       <c r="Z79" t="n">
-        <v>0.42165145495808254</v>
+        <v>0.42165147469479725</v>
       </c>
       <c r="AA79" t="n">
-        <v>0.40786224773645113</v>
+        <v>0.4078624767030761</v>
       </c>
       <c r="AB79" t="n">
-        <v>0.3924767754426619</v>
+        <v>0.3924786061223039</v>
       </c>
       <c r="AC79" t="n">
-        <v>0.3750036640607278</v>
+        <v>0.375008763649696</v>
       </c>
       <c r="AD79" t="n">
-        <v>0.35501116431668545</v>
+        <v>0.3550211476555114</v>
       </c>
       <c r="AE79" t="n">
-        <v>0.32830567022963003</v>
+        <v>0.3283262796986184</v>
       </c>
       <c r="AF79" t="n">
-        <v>0.2874194443954778</v>
+        <v>0.28744589070813137</v>
       </c>
       <c r="AG79" t="n">
-        <v>0.24185571843664122</v>
+        <v>0.24188448975067672</v>
       </c>
       <c r="AH79" t="n">
-        <v>0.1885746232441851</v>
+        <v>0.18860071338861206</v>
       </c>
       <c r="AI79" t="n">
-        <v>0.12749653326554333</v>
+        <v>0.12751191577706267</v>
       </c>
       <c r="AJ79" t="n">
-        <v>0.06151439209813697</v>
+        <v>0.061515345649169384</v>
       </c>
     </row>
   </sheetData>
@@ -41645,21 +41645,23 @@
         <v>0.08374006138180522</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.09554701325527648</v>
+        <v>0.09554700913209575</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.10710879147587808</v>
+        <v>0.10710853746331936</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.11911290112320605</v>
+        <v>0.11911164140760129</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1322150224446215</v>
+        <v>0.13221172269389772</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.14685609592528592</v>
-      </c>
-      <c r="AE5"/>
+        <v>0.1468498219129921</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.16313647951463228</v>
+      </c>
       <c r="AF5"/>
       <c r="AG5"/>
       <c r="AH5"/>
@@ -41743,21 +41745,23 @@
         <v>1.2283031646751872</v>
       </c>
       <c r="Z6" t="n">
-        <v>1.317861520874141</v>
+        <v>1.3178615784752992</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.4034919698923054</v>
+        <v>1.4034952859297214</v>
       </c>
       <c r="AB6" t="n">
-        <v>1.4773426224997488</v>
+        <v>1.4773580581483752</v>
       </c>
       <c r="AC6" t="n">
-        <v>1.53427634807582</v>
+        <v>1.5343144475162491</v>
       </c>
       <c r="AD6" t="n">
-        <v>1.5724306751733588</v>
-      </c>
-      <c r="AE6"/>
+        <v>1.5724991730987399</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1.5932949682023467</v>
+      </c>
       <c r="AF6"/>
       <c r="AG6"/>
       <c r="AH6"/>
@@ -41772,90 +41776,92 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.006444132855484446</v>
+        <v>0.006425614336965928</v>
       </c>
       <c r="D7" t="n">
-        <v>0.006288170238527483</v>
+        <v>0.006269651720008965</v>
       </c>
       <c r="E7" t="n">
-        <v>0.006148330137378747</v>
+        <v>0.0061298116188602285</v>
       </c>
       <c r="F7" t="n">
-        <v>0.006020804166784899</v>
+        <v>0.00600228564826638</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0059111964397340205</v>
+        <v>0.005892677921215502</v>
       </c>
       <c r="H7" t="n">
-        <v>0.005810327337803873</v>
+        <v>0.005791808819285355</v>
       </c>
       <c r="I7" t="n">
-        <v>0.005730117267476682</v>
+        <v>0.005715829275198423</v>
       </c>
       <c r="J7" t="n">
-        <v>0.005660133827335312</v>
+        <v>0.005663799390186647</v>
       </c>
       <c r="K7" t="n">
-        <v>0.005620729657703209</v>
+        <v>0.005642406649162915</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0055904646230869465</v>
+        <v>0.005629898633053762</v>
       </c>
       <c r="M7" t="n">
-        <v>0.005620323409154618</v>
+        <v>0.005635548107949986</v>
       </c>
       <c r="N7" t="n">
-        <v>0.005700422036964881</v>
+        <v>0.005666045990033562</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0057938315052878464</v>
+        <v>0.005793865238187734</v>
       </c>
       <c r="P7" t="n">
-        <v>0.005902561983004892</v>
+        <v>0.005937136141030472</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.006048432101841819</v>
+        <v>0.006091073421285324</v>
       </c>
       <c r="R7" t="n">
-        <v>0.006276667728059033</v>
+        <v>0.00626970007515886</v>
       </c>
       <c r="S7" t="n">
-        <v>0.006516392209908682</v>
+        <v>0.006484346651033734</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0067743349081459394</v>
+        <v>0.006798342384648762</v>
       </c>
       <c r="U7" t="n">
-        <v>0.007058396230076818</v>
+        <v>0.007119160559432684</v>
       </c>
       <c r="V7" t="n">
-        <v>0.00744195770213935</v>
+        <v>0.007456917073749415</v>
       </c>
       <c r="W7" t="n">
-        <v>0.007832714536293845</v>
+        <v>0.007801636965113777</v>
       </c>
       <c r="X7" t="n">
-        <v>0.008241143977504426</v>
+        <v>0.00826236788346106</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.008727817320902696</v>
+        <v>0.008793730036799086</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.009340962880586615</v>
+        <v>0.009346213706051161</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.009967982253366595</v>
+        <v>0.009912122884298148</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.011175296191066997</v>
+        <v>0.011376107652414988</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.015723546695485938</v>
+        <v>0.015666603840148657</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.0171340735462176</v>
-      </c>
-      <c r="AE7"/>
+        <v>0.01872578926725705</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.021711957197527505</v>
+      </c>
       <c r="AF7"/>
       <c r="AG7"/>
       <c r="AH7"/>
@@ -41870,90 +41876,92 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>0.09672276488079745</v>
+        <v>0.09671923264486876</v>
       </c>
       <c r="D8" t="n">
-        <v>0.08477059520479059</v>
+        <v>0.08476706296886191</v>
       </c>
       <c r="E8" t="n">
-        <v>0.07388332863162131</v>
+        <v>0.07387979639569263</v>
       </c>
       <c r="F8" t="n">
-        <v>0.06424397935809724</v>
+        <v>0.06424044712216856</v>
       </c>
       <c r="G8" t="n">
-        <v>0.055664549655323685</v>
+        <v>0.055661017419395005</v>
       </c>
       <c r="H8" t="n">
-        <v>0.04807483623621724</v>
+        <v>0.04807130400028856</v>
       </c>
       <c r="I8" t="n">
-        <v>0.04160167360160434</v>
+        <v>0.041598948299381946</v>
       </c>
       <c r="J8" t="n">
-        <v>0.03646941486927556</v>
+        <v>0.036470114041446886</v>
       </c>
       <c r="K8" t="n">
-        <v>0.032468511355598</v>
+        <v>0.032472646040993224</v>
       </c>
       <c r="L8" t="n">
-        <v>0.029522484440202418</v>
+        <v>0.02953000611245052</v>
       </c>
       <c r="M8" t="n">
-        <v>0.02775156785257079</v>
+        <v>0.02775447182288756</v>
       </c>
       <c r="N8" t="n">
-        <v>0.02736376646389757</v>
+        <v>0.0273572095512625</v>
       </c>
       <c r="O8" t="n">
-        <v>0.028165321647741402</v>
+        <v>0.028165328081979697</v>
       </c>
       <c r="P8" t="n">
-        <v>0.030099003540325884</v>
+        <v>0.0301055982408177</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.03325465320940054</v>
+        <v>0.03326278664623211</v>
       </c>
       <c r="R8" t="n">
-        <v>0.03783150607954892</v>
+        <v>0.03783017706427764</v>
       </c>
       <c r="S8" t="n">
-        <v>0.04363186276057102</v>
+        <v>0.043625750366952744</v>
       </c>
       <c r="T8" t="n">
-        <v>0.05062026655260578</v>
+        <v>0.05062484575644303</v>
       </c>
       <c r="U8" t="n">
-        <v>0.058891213440182215</v>
+        <v>0.0589028036733382</v>
       </c>
       <c r="V8" t="n">
-        <v>0.06860275078176684</v>
+        <v>0.0686056041433799</v>
       </c>
       <c r="W8" t="n">
-        <v>0.0795874316754134</v>
+        <v>0.0795815039164845</v>
       </c>
       <c r="X8" t="n">
-        <v>0.09180204464532968</v>
+        <v>0.0918060929088607</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.10538298612088526</v>
+        <v>0.10539555836110055</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.12042849200568388</v>
+        <v>0.12042949355201939</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.13679286641305954</v>
+        <v>0.1367822117556592</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.15455368328578872</v>
+        <v>0.1545919862125566</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.17435649047574447</v>
+        <v>0.17434562915337123</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.19503258083428174</v>
-      </c>
-      <c r="AE8"/>
+        <v>0.19533618586901927</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.21768136598204998</v>
+      </c>
       <c r="AF8"/>
       <c r="AG8"/>
       <c r="AH8"/>
@@ -41971,87 +41979,89 @@
         <v>5.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4.460352546346369</v>
+        <v>4.460426733076401</v>
       </c>
       <c r="E9" t="n">
-        <v>3.784188773347255</v>
+        <v>3.784355914058529</v>
       </c>
       <c r="F9" t="n">
-        <v>3.094762748642485</v>
+        <v>3.0950246665310166</v>
       </c>
       <c r="G9" t="n">
-        <v>2.3901998301024987</v>
+        <v>2.3905586060762003</v>
       </c>
       <c r="H9" t="n">
-        <v>1.669690758105515</v>
+        <v>1.6701485843233117</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9349279574318565</v>
+        <v>0.9348391844336708</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1869342651015371</v>
+        <v>0.18677438736721808</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.563470592970889</v>
+        <v>-0.5637018046482258</v>
       </c>
       <c r="L9" t="n">
-        <v>-1.3032760377441135</v>
+        <v>-1.3035775757777817</v>
       </c>
       <c r="M9" t="n">
-        <v>-2.0887362244312024</v>
+        <v>-2.088651897466778</v>
       </c>
       <c r="N9" t="n">
-        <v>-2.8753358188844427</v>
+        <v>-2.874750656998505</v>
       </c>
       <c r="O9" t="n">
-        <v>-3.664315252936068</v>
+        <v>-3.6652484696439585</v>
       </c>
       <c r="P9" t="n">
-        <v>-4.456290243803544</v>
+        <v>-4.458747604007552</v>
       </c>
       <c r="Q9" t="n">
-        <v>-5.25349563504682</v>
+        <v>-5.255162677651645</v>
       </c>
       <c r="R9" t="n">
-        <v>-6.057274656298629</v>
+        <v>-6.053117994400685</v>
       </c>
       <c r="S9" t="n">
-        <v>-6.86429956659166</v>
+        <v>-6.86166723607767</v>
       </c>
       <c r="T9" t="n">
-        <v>-7.675071068604764</v>
+        <v>-7.698187104049431</v>
       </c>
       <c r="U9" t="n">
-        <v>-8.500136154557246</v>
+        <v>-8.538441181423963</v>
       </c>
       <c r="V9" t="n">
-        <v>-9.373085747206432</v>
+        <v>-9.381476491331888</v>
       </c>
       <c r="W9" t="n">
-        <v>-10.25045650428665</v>
+        <v>-10.228781460974645</v>
       </c>
       <c r="X9" t="n">
-        <v>-11.132908589008782</v>
+        <v>-11.170818093817545</v>
       </c>
       <c r="Y9" t="n">
-        <v>-12.099211200253674</v>
+        <v>-12.173981111652306</v>
       </c>
       <c r="Z9" t="n">
-        <v>-13.190768187137198</v>
+        <v>-13.18233879051109</v>
       </c>
       <c r="AA9" t="n">
-        <v>-14.290339353098723</v>
+        <v>-14.198096202259087</v>
       </c>
       <c r="AB9" t="n">
-        <v>-16.39205294609279</v>
+        <v>-16.753306482701717</v>
       </c>
       <c r="AC9" t="n">
-        <v>-23.395837312398676</v>
+        <v>-23.31159605477915</v>
       </c>
       <c r="AD9" t="n">
-        <v>-25.0</v>
-      </c>
-      <c r="AE9"/>
+        <v>-26.9218896983961</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>-30.0</v>
+      </c>
       <c r="AF9"/>
       <c r="AG9"/>
       <c r="AH9"/>
@@ -42129,27 +42139,29 @@
         <v>0.4069359553802737</v>
       </c>
       <c r="X10" t="n">
-        <v>0.41066753534460065</v>
+        <v>0.41066753534239486</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.413814199243251</v>
+        <v>0.413814035904988</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.421014007085303</v>
+        <v>0.42100925925324995</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.45046005079671103</v>
+        <v>0.45042623298811746</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.5242443495455548</v>
+        <v>0.5241218930520057</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.6848262802090113</v>
+        <v>0.6844520425109427</v>
       </c>
       <c r="AD10" t="n">
-        <v>1.1811096505816612</v>
-      </c>
-      <c r="AE10"/>
+        <v>1.1795959648966827</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>3.4991923598919126</v>
+      </c>
       <c r="AF10"/>
       <c r="AG10"/>
       <c r="AH10"/>
@@ -42227,27 +42239,29 @@
         <v>-0.15693595538027372</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.16066753534460063</v>
+        <v>-0.16066753534239486</v>
       </c>
       <c r="Y11" t="n">
-        <v>-0.163814199243251</v>
+        <v>-0.16381403590498803</v>
       </c>
       <c r="Z11" t="n">
-        <v>-0.171014007085303</v>
+        <v>-0.17100925925324992</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.200460050796711</v>
+        <v>-0.2004262329881175</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.27424434954555477</v>
+        <v>-0.27412189305200574</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.43482628020901126</v>
+        <v>-0.4344520425109427</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.9311096505816613</v>
-      </c>
-      <c r="AE11"/>
+        <v>-0.9295959648966827</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>-3.2491923598919126</v>
+      </c>
       <c r="AF11"/>
       <c r="AG11"/>
       <c r="AH11"/>
@@ -42262,90 +42276,92 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>-7.950824563805654</v>
+        <v>-7.951114931992198</v>
       </c>
       <c r="D12" t="n">
-        <v>-7.988847105510479</v>
+        <v>-7.989180000054498</v>
       </c>
       <c r="E12" t="n">
-        <v>-7.924843346496178</v>
+        <v>-7.9252222378543475</v>
       </c>
       <c r="F12" t="n">
-        <v>-7.6878794299386435</v>
+        <v>-7.688302144990519</v>
       </c>
       <c r="G12" t="n">
-        <v>-7.22885161420591</v>
+        <v>-7.229310355540126</v>
       </c>
       <c r="H12" t="n">
-        <v>-6.468910363395129</v>
+        <v>-6.4693856930763225</v>
       </c>
       <c r="I12" t="n">
-        <v>-5.280963092394179</v>
+        <v>-5.28130906797867</v>
       </c>
       <c r="J12" t="n">
-        <v>-3.523324591071461</v>
+        <v>-3.5232570450664817</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.1517548302132006</v>
+        <v>-1.1516081792790775</v>
       </c>
       <c r="L12" t="n">
-        <v>1.827523265770434</v>
+        <v>1.827057772096692</v>
       </c>
       <c r="M12" t="n">
-        <v>5.22133544289948</v>
+        <v>5.220789130822751</v>
       </c>
       <c r="N12" t="n">
-        <v>8.615565736082573</v>
+        <v>8.617630694927419</v>
       </c>
       <c r="O12" t="n">
-        <v>11.59238689201876</v>
+        <v>11.592384243791853</v>
       </c>
       <c r="P12" t="n">
-        <v>13.859032150867861</v>
+        <v>13.855996298020484</v>
       </c>
       <c r="Q12" t="n">
-        <v>15.266379428926205</v>
+        <v>15.262646484538456</v>
       </c>
       <c r="R12" t="n">
-        <v>15.810089202546934</v>
+        <v>15.81064462817856</v>
       </c>
       <c r="S12" t="n">
-        <v>15.778731771224528</v>
+        <v>15.78094252562008</v>
       </c>
       <c r="T12" t="n">
-        <v>15.382838762432232</v>
+        <v>15.381447327984656</v>
       </c>
       <c r="U12" t="n">
-        <v>14.752768689928294</v>
+        <v>14.749865805546747</v>
       </c>
       <c r="V12" t="n">
-        <v>13.976680992043953</v>
+        <v>13.976099690770992</v>
       </c>
       <c r="W12" t="n">
-        <v>13.177520214870567</v>
+        <v>13.178501764090806</v>
       </c>
       <c r="X12" t="n">
-        <v>12.40260066881129</v>
+        <v>12.402053766156069</v>
       </c>
       <c r="Y12" t="n">
-        <v>11.6556116873192</v>
+        <v>11.654221333187888</v>
       </c>
       <c r="Z12" t="n">
-        <v>10.943104068860563</v>
+        <v>10.943013539337441</v>
       </c>
       <c r="AA12" t="n">
-        <v>10.259979242297058</v>
+        <v>10.260802687098336</v>
       </c>
       <c r="AB12" t="n">
-        <v>9.558766838108678</v>
+        <v>9.556498330496112</v>
       </c>
       <c r="AC12" t="n">
-        <v>8.799651472046921</v>
+        <v>8.800418197846062</v>
       </c>
       <c r="AD12" t="n">
-        <v>8.062399976696435</v>
-      </c>
-      <c r="AE12"/>
+        <v>8.050219502868575</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>7.3193907113470145</v>
+      </c>
       <c r="AF12"/>
       <c r="AG12"/>
       <c r="AH12"/>
@@ -42360,7 +42376,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>15.810089202546934</v>
+        <v>15.81064462817856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>